<commit_message>
chore: Update generated charts and feedback data
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/classification_feedback.xlsx
+++ b/classification_feedback.xlsx
@@ -705,7 +705,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Generated: 2026-01-30 14:35</t>
+          <t>Generated: 2026-02-03 08:52</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -892,7 +892,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Premature Checkout</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -949,7 +949,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Call Test</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>No Escalation</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Activation</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Invalid CR</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Ignored Anomaly</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Issue</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Issue</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Incomplete Validation</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>Missed Degradation</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>Missed Degradation</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Call Test</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Check</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Market Guideline Violations</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Email/Attachment Issues</t>
+          <t>Wrong Site ID</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>Missed Issue</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>No Escalation</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Issue</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -2317,7 +2317,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Swap</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Wrong Attachment</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Improper Escalations</t>
+          <t>Wrong Escalation</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>Wrong KPIs</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Wrong Nest Type</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Wrong Nest Type</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>Wrong KPIs</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Parameter Impact</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Wrong Attachment</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Market Guideline Violations</t>
+          <t>Improper Extension</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Parameter</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>BH Not Ready</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Improper Escalations</t>
+          <t>Wrong Escalation</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -3115,7 +3115,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Wrong Nest Type</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -3172,7 +3172,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Wrong Nest Type</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>RIOT/FCI Tool Issues</t>
+          <t>KPI Impact</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -3423,7 +3423,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Incomplete Snapshot</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -3742,7 +3742,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Issue</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -3799,7 +3799,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>RIOT/FCI Tool Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -4027,7 +4027,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -4084,7 +4084,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -4312,7 +4312,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -4369,7 +4369,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -4483,7 +4483,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>CIQ/SCF Mismatch</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -4597,7 +4597,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -4654,7 +4654,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -4825,7 +4825,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -4882,7 +4882,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Improper Escalations</t>
+          <t>Wrong Escalation</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -4939,7 +4939,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -5053,7 +5053,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -5110,7 +5110,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>CIQ/SCF Mismatch</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -5224,7 +5224,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>BH Not Ready</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Improper Escalations</t>
+          <t>Wrong Escalation</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -5395,7 +5395,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -5452,7 +5452,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -5509,7 +5509,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -5623,7 +5623,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -5680,7 +5680,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -5737,7 +5737,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -5851,7 +5851,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -5908,7 +5908,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -5965,7 +5965,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -6022,7 +6022,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -6079,7 +6079,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>Material Missing</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -6136,7 +6136,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -6193,7 +6193,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -6250,7 +6250,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Release Procedure Issues</t>
+          <t>Process Violation</t>
         </is>
       </c>
       <c r="E97" t="n">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Release Procedure Issues</t>
+          <t>Process Violation</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -6364,7 +6364,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -6421,7 +6421,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -6478,7 +6478,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -6535,7 +6535,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -6592,7 +6592,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Missing Nesting</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -6649,7 +6649,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -6706,7 +6706,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -6820,7 +6820,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Missing Config</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -6934,7 +6934,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>Material Missing</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -6991,7 +6991,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -7048,7 +7048,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -7105,7 +7105,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -7162,7 +7162,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -7219,7 +7219,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -7276,7 +7276,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -7333,7 +7333,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>MW/Transmission Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -7390,7 +7390,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -7447,7 +7447,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -7504,7 +7504,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -7561,7 +7561,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -7618,7 +7618,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>RFDS Mismatch</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -7675,7 +7675,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -7732,7 +7732,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>Material Missing</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -7789,7 +7789,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -7846,7 +7846,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -7903,7 +7903,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -7960,7 +7960,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -8017,7 +8017,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E128" t="n">
@@ -8074,7 +8074,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -8131,7 +8131,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -8188,7 +8188,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Premature Denial</t>
         </is>
       </c>
       <c r="E131" t="n">
@@ -8245,7 +8245,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Deliverable</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -8302,7 +8302,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -8359,7 +8359,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -8416,7 +8416,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -8473,7 +8473,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -8530,7 +8530,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E137" t="n">
@@ -8587,7 +8587,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>TAC Mismatch</t>
         </is>
       </c>
       <c r="E138" t="n">
@@ -8644,7 +8644,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -8701,7 +8701,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>BH Not Ready</t>
         </is>
       </c>
       <c r="E140" t="n">
@@ -8758,7 +8758,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E141" t="n">
@@ -8815,7 +8815,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E142" t="n">
@@ -8872,7 +8872,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E143" t="n">
@@ -8929,7 +8929,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E144" t="n">
@@ -8986,7 +8986,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E145" t="n">
@@ -9043,7 +9043,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E146" t="n">
@@ -9100,7 +9100,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E147" t="n">
@@ -9157,7 +9157,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E148" t="n">
@@ -9214,7 +9214,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E149" t="n">
@@ -9271,7 +9271,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>BH Check Error</t>
         </is>
       </c>
       <c r="E150" t="n">
@@ -9328,7 +9328,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>No Reversion</t>
         </is>
       </c>
       <c r="E151" t="n">
@@ -9385,7 +9385,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E152" t="n">
@@ -9442,7 +9442,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E153" t="n">
@@ -9465,7 +9465,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E154" t="n">
@@ -9556,7 +9556,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E155" t="n">
@@ -9613,7 +9613,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>RIOT/FCI Tool Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E156" t="n">
@@ -9636,7 +9636,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
@@ -9670,7 +9670,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>RFDS Mismatch</t>
         </is>
       </c>
       <c r="E157" t="n">
@@ -9784,7 +9784,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>MW/Transmission Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E159" t="n">
@@ -9841,7 +9841,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E160" t="n">
@@ -9898,7 +9898,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E161" t="n">
@@ -9955,7 +9955,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E162" t="n">
@@ -10012,7 +10012,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E163" t="n">
@@ -10069,7 +10069,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E164" t="n">
@@ -10092,7 +10092,7 @@
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
@@ -10126,7 +10126,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E165" t="n">
@@ -10183,7 +10183,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E166" t="n">
@@ -10240,7 +10240,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E167" t="n">
@@ -10297,7 +10297,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>BH Not Ready</t>
         </is>
       </c>
       <c r="E168" t="n">
@@ -10354,7 +10354,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>Material Missing</t>
         </is>
       </c>
       <c r="E169" t="n">
@@ -10411,7 +10411,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E170" t="n">
@@ -10468,7 +10468,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E171" t="n">
@@ -10525,7 +10525,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E172" t="n">
@@ -10582,7 +10582,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Site Down</t>
         </is>
       </c>
       <c r="E173" t="n">
@@ -10639,7 +10639,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>RFDS Mismatch</t>
         </is>
       </c>
       <c r="E174" t="n">
@@ -10696,7 +10696,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E175" t="n">
@@ -10753,7 +10753,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>TAC Mismatch</t>
         </is>
       </c>
       <c r="E176" t="n">
@@ -10810,7 +10810,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E177" t="n">
@@ -10867,7 +10867,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Wrong Site ID</t>
         </is>
       </c>
       <c r="E178" t="n">
@@ -10924,7 +10924,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Wrong Site ID</t>
         </is>
       </c>
       <c r="E179" t="n">
@@ -10981,7 +10981,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Wrong Site ID</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -11004,7 +11004,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
@@ -11038,7 +11038,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E181" t="n">
@@ -11095,7 +11095,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Release Procedure Issues</t>
+          <t>Process Violation</t>
         </is>
       </c>
       <c r="E182" t="n">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
@@ -11152,7 +11152,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Release Procedure Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E183" t="n">
@@ -11209,7 +11209,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Release Procedure Issues</t>
+          <t>Process Violation</t>
         </is>
       </c>
       <c r="E184" t="n">
@@ -11266,7 +11266,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Process Skip</t>
         </is>
       </c>
       <c r="E185" t="n">
@@ -11289,7 +11289,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
@@ -11323,7 +11323,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E186" t="n">
@@ -11380,7 +11380,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E187" t="n">
@@ -11437,7 +11437,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E188" t="n">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E189" t="n">
@@ -11551,7 +11551,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E190" t="n">
@@ -11608,7 +11608,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E191" t="n">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -11665,7 +11665,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E192" t="n">
@@ -11722,7 +11722,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E193" t="n">
@@ -11779,7 +11779,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E194" t="n">
@@ -11802,7 +11802,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>19%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
@@ -11836,7 +11836,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>One-T Mismatch</t>
         </is>
       </c>
       <c r="E195" t="n">
@@ -11893,7 +11893,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>One-T Mismatch</t>
         </is>
       </c>
       <c r="E196" t="n">
@@ -11950,7 +11950,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E197" t="n">
@@ -12007,7 +12007,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>One-T Mismatch</t>
         </is>
       </c>
       <c r="E198" t="n">
@@ -12064,7 +12064,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Missing Documents</t>
         </is>
       </c>
       <c r="E199" t="n">
@@ -12121,7 +12121,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E200" t="n">
@@ -12178,7 +12178,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E201" t="n">
@@ -12235,7 +12235,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E202" t="n">
@@ -12292,7 +12292,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E203" t="n">
@@ -12349,7 +12349,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E204" t="n">
@@ -12406,7 +12406,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E205" t="n">
@@ -12463,7 +12463,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E206" t="n">
@@ -12520,7 +12520,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E207" t="n">
@@ -12577,7 +12577,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E208" t="n">
@@ -12634,7 +12634,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E209" t="n">
@@ -12714,7 +12714,7 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J210" t="inlineStr">
@@ -12748,7 +12748,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E211" t="n">
@@ -12805,7 +12805,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Swap</t>
         </is>
       </c>
       <c r="E212" t="n">
@@ -12862,7 +12862,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E213" t="n">
@@ -12976,7 +12976,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E215" t="n">
@@ -13033,7 +13033,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>Design Mismatch</t>
         </is>
       </c>
       <c r="E216" t="n">
@@ -13090,7 +13090,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Missing Documents</t>
         </is>
       </c>
       <c r="E217" t="n">
@@ -13147,7 +13147,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E218" t="n">
@@ -13204,7 +13204,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>MW/Transmission Issues</t>
+          <t>MW Not Ready</t>
         </is>
       </c>
       <c r="E219" t="n">
@@ -13318,7 +13318,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E221" t="n">
@@ -13375,7 +13375,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E222" t="n">
@@ -13432,7 +13432,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="E223" t="n">
@@ -13489,7 +13489,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E224" t="n">
@@ -13546,7 +13546,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E225" t="n">
@@ -13603,7 +13603,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E226" t="n">
@@ -13660,7 +13660,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E227" t="n">
@@ -13717,7 +13717,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E228" t="n">
@@ -13774,7 +13774,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E229" t="n">
@@ -13831,7 +13831,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E230" t="n">
@@ -13888,7 +13888,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Closeout/Bucket Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E231" t="n">
@@ -13945,7 +13945,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E232" t="n">
@@ -14002,7 +14002,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E233" t="n">
@@ -14059,7 +14059,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E234" t="n">
@@ -14116,7 +14116,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E235" t="n">
@@ -14173,7 +14173,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E236" t="n">
@@ -14230,7 +14230,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E237" t="n">
@@ -14287,7 +14287,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E238" t="n">
@@ -14344,7 +14344,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E239" t="n">
@@ -14401,7 +14401,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E240" t="n">
@@ -14458,7 +14458,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>Spectrum Mismatch</t>
         </is>
       </c>
       <c r="E241" t="n">
@@ -14515,7 +14515,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E242" t="n">
@@ -14572,7 +14572,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E243" t="n">
@@ -14629,7 +14629,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E244" t="n">
@@ -14686,7 +14686,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E245" t="n">
@@ -14743,7 +14743,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E246" t="n">
@@ -14800,7 +14800,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E247" t="n">
@@ -14857,7 +14857,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>RFDS Mismatch</t>
         </is>
       </c>
       <c r="E248" t="n">
@@ -14914,7 +14914,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>TAC Mismatch</t>
         </is>
       </c>
       <c r="E249" t="n">
@@ -14971,7 +14971,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E250" t="n">
@@ -15028,7 +15028,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E251" t="n">
@@ -15085,7 +15085,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Missed Call Test</t>
         </is>
       </c>
       <c r="E252" t="n">
@@ -15142,7 +15142,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E253" t="n">
@@ -15165,7 +15165,7 @@
       </c>
       <c r="I253" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J253" t="inlineStr">
@@ -15222,7 +15222,7 @@
       </c>
       <c r="I254" t="inlineStr">
         <is>
-          <t>22%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J254" t="inlineStr">
@@ -15313,7 +15313,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Snapshot</t>
         </is>
       </c>
       <c r="E256" t="n">
@@ -15370,7 +15370,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Snapshot</t>
         </is>
       </c>
       <c r="E257" t="n">
@@ -15393,7 +15393,7 @@
       </c>
       <c r="I257" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J257" t="inlineStr">
@@ -15427,7 +15427,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E258" t="n">
@@ -15484,7 +15484,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E259" t="n">
@@ -15541,7 +15541,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>No Proactive Update</t>
         </is>
       </c>
       <c r="E260" t="n">
@@ -15598,7 +15598,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Process Skip</t>
         </is>
       </c>
       <c r="E261" t="n">
@@ -15655,7 +15655,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Email/Attachment Issues</t>
+          <t>Wrong Subject</t>
         </is>
       </c>
       <c r="E262" t="n">
@@ -15769,7 +15769,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>BH Not Ready</t>
         </is>
       </c>
       <c r="E264" t="n">
@@ -15826,7 +15826,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Email/Attachment Issues</t>
+          <t>Wrong Site ID</t>
         </is>
       </c>
       <c r="E265" t="n">
@@ -15883,7 +15883,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E266" t="n">
@@ -15997,7 +15997,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E268" t="n">
@@ -16054,7 +16054,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E269" t="n">
@@ -16111,7 +16111,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E270" t="n">
@@ -16168,7 +16168,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E271" t="n">
@@ -16225,7 +16225,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Closeout/Bucket Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E272" t="n">
@@ -16282,7 +16282,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Closeout/Bucket Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E273" t="n">
@@ -16339,7 +16339,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Missing Documents</t>
         </is>
       </c>
       <c r="E274" t="n">
@@ -16396,7 +16396,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Missing Snapshot</t>
         </is>
       </c>
       <c r="E275" t="n">
@@ -16453,7 +16453,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E276" t="n">
@@ -16510,7 +16510,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E277" t="n">
@@ -16567,7 +16567,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E278" t="n">
@@ -16624,7 +16624,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E279" t="n">
@@ -16681,7 +16681,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E280" t="n">
@@ -16738,7 +16738,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E281" t="n">
@@ -16795,7 +16795,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E282" t="n">
@@ -16852,7 +16852,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E283" t="n">
@@ -16909,7 +16909,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Closeout/Bucket Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E284" t="n">
@@ -16966,7 +16966,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E285" t="n">
@@ -17023,7 +17023,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E286" t="n">
@@ -17080,7 +17080,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E287" t="n">
@@ -17137,7 +17137,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E288" t="n">
@@ -17194,7 +17194,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>MW/Transmission Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E289" t="n">
@@ -17251,7 +17251,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>IP Mismatch</t>
         </is>
       </c>
       <c r="E290" t="n">
@@ -17308,7 +17308,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E291" t="n">
@@ -17365,7 +17365,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>MW/Transmission Issues</t>
+          <t>MW Not Ready</t>
         </is>
       </c>
       <c r="E292" t="n">
@@ -17422,7 +17422,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E293" t="n">
@@ -17479,7 +17479,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E294" t="n">
@@ -17536,7 +17536,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E295" t="n">
@@ -17593,7 +17593,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E296" t="n">
@@ -17650,7 +17650,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>Site Down</t>
         </is>
       </c>
       <c r="E297" t="n">
@@ -17707,7 +17707,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E298" t="n">
@@ -17844,7 +17844,7 @@
       </c>
       <c r="I300" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="J300" t="inlineStr">
@@ -18015,7 +18015,7 @@
       </c>
       <c r="I303" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J303" t="inlineStr">
@@ -18072,7 +18072,7 @@
       </c>
       <c r="I304" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J304" t="inlineStr">
@@ -18106,7 +18106,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>One-T Mismatch</t>
         </is>
       </c>
       <c r="E305" t="n">
@@ -18129,7 +18129,7 @@
       </c>
       <c r="I305" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>17%</t>
         </is>
       </c>
       <c r="J305" t="inlineStr">
@@ -18163,7 +18163,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E306" t="n">
@@ -18220,7 +18220,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E307" t="n">
@@ -18277,7 +18277,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E308" t="n">
@@ -18334,7 +18334,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E309" t="n">
@@ -18391,7 +18391,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E310" t="n">
@@ -18448,7 +18448,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E311" t="n">
@@ -18471,7 +18471,7 @@
       </c>
       <c r="I311" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J311" t="inlineStr">
@@ -18562,7 +18562,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>Missing Config</t>
         </is>
       </c>
       <c r="E313" t="n">
@@ -18619,7 +18619,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>Config Error</t>
         </is>
       </c>
       <c r="E314" t="n">
@@ -18642,7 +18642,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>17%</t>
         </is>
       </c>
       <c r="J314" t="inlineStr">
@@ -18676,7 +18676,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E315" t="n">
@@ -18733,7 +18733,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>MW/Transmission Issues</t>
+          <t>MW Not Ready</t>
         </is>
       </c>
       <c r="E316" t="n">
@@ -18790,7 +18790,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Repeated Queries</t>
         </is>
       </c>
       <c r="E317" t="n">
@@ -18813,7 +18813,7 @@
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J317" t="inlineStr">
@@ -18870,7 +18870,7 @@
       </c>
       <c r="I318" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J318" t="inlineStr">
@@ -18961,7 +18961,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="E320" t="n">
@@ -19018,7 +19018,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Missing Snapshot</t>
         </is>
       </c>
       <c r="E321" t="n">
@@ -19075,7 +19075,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E322" t="n">
@@ -19189,7 +19189,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>IP Mismatch</t>
         </is>
       </c>
       <c r="E324" t="n">
@@ -19212,7 +19212,7 @@
       </c>
       <c r="I324" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J324" t="inlineStr">
@@ -19246,7 +19246,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="E325" t="n">
@@ -19360,7 +19360,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E327" t="n">
@@ -19417,7 +19417,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E328" t="n">
@@ -19474,7 +19474,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E329" t="n">
@@ -19531,7 +19531,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E330" t="n">
@@ -19588,7 +19588,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Release Procedure Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E331" t="n">
@@ -19645,7 +19645,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E332" t="n">
@@ -19702,7 +19702,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Wrong Nest Type</t>
         </is>
       </c>
       <c r="E333" t="n">
@@ -19759,7 +19759,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E334" t="n">
@@ -19873,7 +19873,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E336" t="n">
@@ -19930,7 +19930,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E337" t="n">
@@ -19987,7 +19987,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E338" t="n">
@@ -20010,7 +20010,7 @@
       </c>
       <c r="I338" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J338" t="inlineStr">
@@ -20044,7 +20044,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E339" t="n">
@@ -20158,7 +20158,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E341" t="n">
@@ -20215,7 +20215,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Follow-up Issues</t>
+          <t>Delayed Response</t>
         </is>
       </c>
       <c r="E342" t="n">
@@ -20272,7 +20272,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Rework</t>
         </is>
       </c>
       <c r="E343" t="n">
@@ -20329,7 +20329,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Wrong Nest Type</t>
         </is>
       </c>
       <c r="E344" t="n">
@@ -20386,7 +20386,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Follow-up Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E345" t="n">
@@ -20443,7 +20443,7 @@
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E346" t="n">
@@ -20500,7 +20500,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E347" t="n">
@@ -20557,7 +20557,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Config Error</t>
         </is>
       </c>
       <c r="E348" t="n">
@@ -20614,7 +20614,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E349" t="n">
@@ -20785,7 +20785,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E352" t="n">
@@ -20899,7 +20899,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E354" t="n">
@@ -20956,7 +20956,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>Incomplete Testing</t>
         </is>
       </c>
       <c r="E355" t="n">
@@ -21013,7 +21013,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>Closeout/Bucket Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E356" t="n">
@@ -21070,7 +21070,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E357" t="n">
@@ -21127,7 +21127,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>BH Status Issue</t>
         </is>
       </c>
       <c r="E358" t="n">
@@ -21150,7 +21150,7 @@
       </c>
       <c r="I358" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J358" t="inlineStr">
@@ -21184,7 +21184,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="E359" t="n">
@@ -21241,7 +21241,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>Material Missing</t>
         </is>
       </c>
       <c r="E360" t="n">
@@ -21298,7 +21298,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E361" t="n">
@@ -21355,7 +21355,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E362" t="n">
@@ -21412,7 +21412,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Port Matrix Mismatch</t>
         </is>
       </c>
       <c r="E363" t="n">
@@ -21435,7 +21435,7 @@
       </c>
       <c r="I363" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J363" t="inlineStr">
@@ -21469,7 +21469,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>Closeout/Bucket Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E364" t="n">
@@ -21526,7 +21526,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Missing Snapshot</t>
         </is>
       </c>
       <c r="E365" t="n">
@@ -21583,7 +21583,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Missing Snapshot</t>
         </is>
       </c>
       <c r="E366" t="n">
@@ -21606,7 +21606,7 @@
       </c>
       <c r="I366" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J366" t="inlineStr">
@@ -21640,7 +21640,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Incorrect Status</t>
         </is>
       </c>
       <c r="E367" t="n">
@@ -21697,7 +21697,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Missed Tech</t>
         </is>
       </c>
       <c r="E368" t="n">
@@ -21720,7 +21720,7 @@
       </c>
       <c r="I368" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J368" t="inlineStr">
@@ -21754,7 +21754,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E369" t="n">
@@ -21811,7 +21811,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>RFDS Mismatch</t>
         </is>
       </c>
       <c r="E370" t="n">
@@ -21868,7 +21868,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Incorrect Status</t>
         </is>
       </c>
       <c r="E371" t="n">
@@ -21925,7 +21925,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>RFDS Mismatch</t>
         </is>
       </c>
       <c r="E372" t="n">
@@ -21982,7 +21982,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E373" t="n">
@@ -22039,7 +22039,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>TAC Mismatch</t>
         </is>
       </c>
       <c r="E374" t="n">
@@ -22096,7 +22096,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>TAC Mismatch</t>
         </is>
       </c>
       <c r="E375" t="n">
@@ -22153,7 +22153,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missed Call Test</t>
         </is>
       </c>
       <c r="E376" t="n">
@@ -22210,7 +22210,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E377" t="n">
@@ -22267,7 +22267,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="E378" t="n">
@@ -22586,7 +22586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22619,12 +22619,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TI/Calendar Issues</t>
+          <t>No TI Entry</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TI, Ti, calendar, TI entry missing, not in TI</t>
+          <t>not schedule in Ti, TI entry missing, not in TI, not in Ti, schedule missing in Ti</t>
         </is>
       </c>
     </row>
@@ -22636,12 +22636,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FE Coordination</t>
+          <t>Schedule Not Followed</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>FE on site, FE logged, logged for IX, logged for support, FE logged in for integration</t>
+          <t>schedule not followed, Site schedule for, but FE logged, FE didn't login, schedule for IX on</t>
         </is>
       </c>
     </row>
@@ -22653,46 +22653,46 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Closeout/Bucket Issues</t>
+          <t>Weekend Schedule Issue</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>closeout, close out, ticket in closeout, moved to closeout, wrong bucket</t>
+          <t>weekend, not site schedule on weekend, over weekend, not schedule on weekend, site schedule on weekend</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Documentation &amp; Reporting</t>
+          <t>Scheduling &amp; Planning</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Snapshot/Screenshot Issues</t>
+          <t>Ticket Status Issue</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>snapshot, snap, screenshot, missing snapshot, snapshot missing</t>
+          <t>closeout, close out, ticket in closeout, Ticket was in closeout, moved to closeout</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Documentation &amp; Reporting</t>
+          <t>Scheduling &amp; Planning</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>E911/CBN Reports</t>
+          <t>Premature Scheduling</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CBN, E911, CBN output missing, E911 Go mail, E911 complete mail</t>
+          <t>without microwave ready, without BH ready, BH not ready, schedule without, MW not ready</t>
         </is>
       </c>
     </row>
@@ -22704,318 +22704,1423 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Email/Attachment Issues</t>
+          <t>Missing Snapshot</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>attachment, email, mail, subject, wrong site ID</t>
+          <t>snapshot missing, missing snapshot, CBN snapshot missing, snapshot is missing, snap missing</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Validation &amp; QA</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Precheck/Postcheck Failures</t>
+          <t>Missing Attachment</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>precheck, postcheck, validation, incomplete validation, missed to check</t>
+          <t>missed to attach, forgot to attach, missing attachment, not attached, attachment missing</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Validation &amp; QA</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Measurement Issues</t>
+          <t>Incorrect Reporting</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>VSWR, RSSI, RTWP, KPI, pass</t>
+          <t>incorrectly, RTT from IX vendor was also wrong, didn't provide a clear view, wrong which, reporting</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Validation &amp; QA</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Escalation Gaps</t>
+          <t>Missing Logs</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>escalated, issue not escalated, missed to escalate, alarm captured but not, not detected</t>
+          <t>forgets to paste, manual logs, missing logs, no logs populated, logs missing</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Process Compliance</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SOP Violations</t>
+          <t>Wrong Attachment</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SOP, process, guideline, not following process, not following SOP</t>
+          <t>wrong attachment, wrongly attached, different site, another site, Detailed site view snap</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Process Compliance</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Improper Escalations</t>
+          <t>Wrong Site ID</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>escalate, NTAC, escalated to NTAC, improper escalation, escalated to NTAC while not supposed to</t>
+          <t>wrong site ID, different site id, Wrong site id, mistakenly placed a different site, site ID missing</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Process Compliance</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Release Procedure Issues</t>
+          <t>Incorrect Status</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>released without, supported without, without BH actualized, without backhaul, bypassed validation</t>
+          <t>marked VSWR as Fail, actual status is, incorrect information, marked as Pass, but actual</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Configuration &amp; Data Mismatch</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Port Matrix Issues</t>
+          <t>Incomplete Snapshot</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>port matrix, PMX, port matrix mismatch, need updated port matrix, as per port matrix</t>
+          <t>Incomplete lemming snapshot, incomplete snapshot, only 2 sectors, sector was missing, In-complete</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Configuration &amp; Data Mismatch</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RET/TAC Naming</t>
+          <t>Data Mismatch</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>RET, TAC, naming, RET naming issue, RET naming wrong</t>
+          <t>mentioned different, as compared to, mismatch, Count of sectors mentioned different</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Configuration &amp; Data Mismatch</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SCF/CIQ/RFDS Mismatch</t>
+          <t>Missing Information</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SCF, CIQ, RFDS, SCF mismatch, CIQ mismatch</t>
+          <t>PSAP contact missing, Table with PSAP, missing, not available, missing in mail</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Site Readiness</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Backhaul Issues</t>
+          <t>Wrong Subject</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>BH, backhaul, actualized, BH not actualized, backhaul not ready</t>
+          <t>subject line, Subject should have been, wrong subject</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Site Readiness</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MW/Transmission Issues</t>
+          <t>Process Skip</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MW, microwave, MW not ready, microwave not ready, MW link was not ready</t>
+          <t>without sending, E911 completion mail circulated, without E911 Go mail, skipped</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Site Readiness</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Material/Equipment Issues</t>
+          <t>Missing Deliverable</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>material, SFP, material missing, SFP missing, site was down</t>
+          <t>RTT wasn't released, EOD released, not released, released later</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Communication &amp; Response</t>
+          <t>Validation &amp; QA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Delayed Responses</t>
+          <t>Premature Checkout</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>delay, delayed, delayed reply, delayed response, delay in reply</t>
+          <t>checked out GC, Logged the GC out, cells were locked, premature checkout, early checkout</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Communication &amp; Response</t>
+          <t>Validation &amp; QA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Follow-up Issues</t>
+          <t>Incomplete Validation</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>follow-up, reminder, follow-up required, multiple follow-ups, reminder sent</t>
+          <t>without checking, IX precheck without, not updated, incomplete validation, BH fields</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Communication &amp; Response</t>
+          <t>Validation &amp; QA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Distro/Routing Issues</t>
+          <t>Invalid CR</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>distro, wrong distro, communication gap, not communicated, proactive update missing</t>
+          <t>Invalid CR, invalid CR manually, wrong CR</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Nesting &amp; Tool Errors</t>
+          <t>Validation &amp; QA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nesting Type Errors</t>
+          <t>Ignored Anomaly</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>nested, nesting, NSA, NSI, nested as NSA</t>
+          <t>anomaly detection, left max tilt, even though it was captured, ignored anomaly, max tilt values</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nesting &amp; Tool Errors</t>
+          <t>Validation &amp; QA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RIOT/FCI Tool Issues</t>
+          <t>Missed Issue</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>RIOT, FCI, RIOT red, RIOT mismatch, tool not updated</t>
+          <t>did not report, Miss to capture, missed to create, Engineer did not identified, missed to attach</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Wrong Denial</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>denied for Anchor site, IX precheck denied, wrong BH validation, BH was already actualized</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Missed Activation</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>VONR is not activated, not activated, missed activation</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Missed Check</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Miss to check, Cell Status Verification, cells were in Unsync, missed to check</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>No Escalation</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>not escalated, but not escalated, no escalation, captured but not escalated</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Wrong KPIs</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>different set of KPIs, wrong KPIs, not aligned with the agreed</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Missed Degradation</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>degradation was not detected, locked and showing zero traffic, missed degradation, not detected during</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Skipped Validation</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>moved to Post check without, skipped validation, without Riot lemming validation</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Wrong Tool Usage</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>AEHC swap report, tool will only flag, wrong tool, Does Not Recognize Physical Swap</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Premature Denial</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>IX support was denied, despite BH status, citing the reason, TI record was not updated, denied support</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Incomplete Testing</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>missing L21 Gamma, VoNR testing, call test, calls were completed and passed, incomplete testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Missed Call Test</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>AWS3 E911 call test, missed, released full RTT, caught during audit, schedule FE for call test</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>No Reversion</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>did not revert, original values, no reversion, tilt settings, not reverted</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Validation &amp; QA</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Missed Tech</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>N6 was missed, missed to add, NSD site, revisit for CT</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Missed Step</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>missed to share, missed to unlock, Engineer missed, missed step, didn't lock the cells</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>No Escalation</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>not escalated to concerned, created the issue ticket but not, no escalation, not escalated</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Wrong Escalation</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>escalated to different vendor, wrong distro, escalated to NTAC, which is raised by client, wrong escalation</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Wrong Bucket</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>not in correct bucket, wrong bucket, Preliminary design, Ticket is not created, ticket was in Design phase</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Process Violation</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>IX supported without, without Backhaul acceptance, released by PAG BO without, BH not actualized, process violation</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Missing Ticket</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ticket not created, Ticket is not created, PAG ticket, not created for the site, missing ticket</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Wrong Nest State</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>sector swap started by GC with site nested in NSI, wrong nest state, nested in</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Wrong File Used</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>some other file was used, wrong file, correct SCF, during integration some other</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Missed Guidance</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>could have informed FE, if PSAP was busy, whitelisted in lieu of, missed guidance</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Process Compliance</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Process Non-Compliance</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>adhere to the guidelines, inquiries from, Tool Request Submission Process, non-compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>RET Naming</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>RET naming issue, RET naming, extra '2', inadvertently removed I, RET naming mismatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>RET Swap</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>RET naming swap, swapped, RET swap, controlling unit, Beta &amp; Gamma</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>RET Parameter</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>RET found Max, max tilt, RET parameter</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Port Matrix Mismatch</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>port matrix, Port Matrix, PMX, Incorrect Port matrix, port matrix mismatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CIQ/SCF Mismatch</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>CIQ and SCF, SCF mismatch, CIQ mismatch, Mismatch in Spectrum sheet, SCF provided with</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TAC Mismatch</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>TAC mismatch, TAC showing mismatched, RIOT red, TAC was, MB TAC</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>RFDS Mismatch</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>RFDS, Mismatch of SCF, RFDS mismatch, SCF and RFDS mismatch, RFDS not mention</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>One-T Mismatch</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>One-T, OneT, One-T not yet updated, One-T mismatch, IP exports</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Design Mismatch</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Design change, HW available on site, ASIA, RFDS with ASIB, design mismatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Missing Documents</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>RFDS &amp; Port Matrix is missing, Port Matrix is missing in TI, missing in TI, missing documents</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Config Error</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Config Error, configuration error, error due to, NRPLMNSET not define, enbid</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Missing Config</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>BWP missing, feature was not activated, missing config, MOCN, Scripts were not implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>IP Mismatch</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>IP mismatch, Gateway IP different, wrong ip, IP different, One-T and SCF</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Spectrum Mismatch</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ARFCN and bandwidth, spectrum plan, spectrum mismatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>BH Not Ready</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>BH not ready, backhaul not ready, BH was not ready, backhaul acceptance, BH readiness pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>MW Not Ready</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>MW not ready, microwave not ready, Microwave link was not ready, MW link was not ready, incomplete microwave</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Material Missing</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>material missing, SFP missing, AMID not available, missing material, Material</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Site Down</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>site was down, shut down, Site was shut down, couldn't lock the live cells, site down</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Site Complexity</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>middle of a microwave chain, downstream sites, didn't have CRs, generator, complexity</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>iNTP Not Ready</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>iNTP still not completed, iNTP not ready</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>BH Check Error</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>BH readiness, checked wrongly, BH Check Error, wrong method, mistake</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Site Readiness</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>BH Status Issue</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>BH Actualization filled as pending, BH pending in field, BH status, status issue</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Communication &amp; Response</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Delayed Response</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Delay in reply, Delayed reply, delayed response, GC query, Replied back</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Communication &amp; Response</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Delayed Deliverable</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>FE waited, waiting for, hrs to get EOD, 3hrs, 4hrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Communication &amp; Response</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>No Proactive Update</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>pro-actively, questioned why, such queries, getting questioned over delays, proactive update</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Communication &amp; Response</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>No Proactive Communication</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>could have communicated, not completed on Friday, Had to cancel, Else could have, proactive communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Communication &amp; Response</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Repeated Queries</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>same queries, new IX BO engg, each day, unnecessary delays, repeated queries</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Communication &amp; Response</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>No Communication</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>No information, schedule from PM to FE, not communicated, no communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Communication &amp; Response</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Training Issue</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>FE doesn't know, Competency issue, even after explaining, training issue, doesn't know how</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
           <t>Nesting &amp; Tool Errors</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Market Guideline Violations</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>market, guideline, not allowed in market, market guideline, nest extended</t>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Wrong Nest Type</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>nested as NSA, nested as SA, nested as NSI, wrong nest type, which is not allowed</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Improper Extension</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>nest extended, extended the nest, nest extension, during Follow Up, improper extension</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Missing Nesting</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>not Nested, was not added in Nesting tool, without Nesting, missing nesting</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Parameter Impact</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>NR UL traffic volume reduction, shifted to LTE, post site modification, parameter impact</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>KPI Impact</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>TPUT decrease, Cluster KPI, KPI impact, degraded, post</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Neighbor Impact</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>starts to deviate, MS2 site, on-aired, neighbor impact</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Missed Activation</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>VONR was not activated, despite requested, only NRPCI was shared, missed activation</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Post-OA Degradation</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>congestion, low Throughput, AFR, DCR degraded, HSI low speed</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Alarm Naming</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>External alarm, naming is incorrect, SURGE SUPPRESSOR, alarm naming</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Delayed Audit</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Audit after 5days, delay in Audit, delayed audit</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Rework</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>rework, PM again requesting, why, was deleted, no clarity</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>HW Issue</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>GPS SFP, PTP sync issue, RET Antenna control failure, hardware fault, antenna will be replaced</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Premature Unlock</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>unlocked the cells, change the cell status to UUU, pending with call test, premature unlock</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>External Cancel</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Site was cancelled, TMO didnt want, Holiday week, external cancel</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Update generated charts and data files
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/classification_feedback.xlsx
+++ b/classification_feedback.xlsx
@@ -705,7 +705,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Generated: 2026-02-03 08:52</t>
+          <t>Generated: 2026-02-04 12:37</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M378"/>
+  <dimension ref="A1:M390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -825,7 +825,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CBN - the snapshot N25_1c_Alpha is missing, despite the fact he validated correctly as PASS.</t>
+          <t>the snapshot N25_1c_Alpha is missing, despite the fact he validated correctly as PASS.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -848,17 +848,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>31%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -882,21 +882,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PostCheck - Engineer Logged the GC out even though cells were locked on site.</t>
+          <t>Engineer Logged the GC out even though cells were locked on site.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Validation &amp; QA</t>
+          <t>Scheduling &amp; Planning</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Premature Checkout</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.621</v>
+        <v>0.663</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -905,7 +905,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -915,7 +915,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BO Support Delays - engineer missed to share IX precheck on E// site.</t>
+          <t>engineer missed to share IX precheck on E// site.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PostCheck - Rets were disabled during check-out and GC was not responding the call. Engineer created the issue ticket but not escalated to concerned stakeholders.</t>
+          <t>Rets were disabled during check-out and GC was not responding the call. Engineer created the issue ticket but not escalated to concerned stakeholders.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.62</v>
+        <v>0.586</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1024,12 +1024,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1053,21 +1053,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Audits - VONR is not activated on Site during CBN Validations</t>
+          <t>VONR is not activated on Site during CBN Validations</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Validation &amp; QA</t>
+          <t>Configuration &amp; Data Mismatch</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Missed Activation</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.616</v>
+        <v>0.633</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PreCheck - engineer shared IX precheck without checking the backhaul columns on MagentaBuilt</t>
+          <t>engineer shared IX precheck without checking the backhaul columns on MagentaBuilt</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PreCheck - engineer shared IX precheck without checking the backhaul columns on MagentaBuilt</t>
+          <t>engineer shared IX precheck without checking the backhaul columns on MagentaBuilt</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1224,21 +1224,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PreCheck - Engineer moved PCI ticket to Nest with Invalid CR manually.</t>
+          <t>Engineer moved PCI ticket to Nest with Invalid CR manually.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Validation &amp; QA</t>
+          <t>Nesting &amp; Tool Errors</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Invalid CR</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.648</v>
+        <v>0.632</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1252,12 +1252,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PostCheck - During the post check the RETs are in max tilt, and PAG engineer checked out GC as the site left max tilt values even though it was captured in anomaly detection</t>
+          <t>During the post check the RETs are in max tilt, and PAG engineer checked out GC as the site left max tilt values even though it was captured in anomaly detection</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1304,17 +1304,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PreCheck - Engineer missed to attach Pre-check logs in the ticket</t>
+          <t>Engineer missed to attach Pre-check logs in the ticket</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>PostCheck - The issue is that the engineer did not report the RSSI case with an exact 3 dB imbalance.</t>
+          <t>The issue is that the engineer did not report the RSSI case with an exact 3 dB imbalance.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1409,7 +1409,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.61</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PreCheck - Engineer released IX precheck while BH fields of MB were not updated</t>
+          <t>Engineer released IX precheck while BH fields of MB were not updated</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1466,7 +1466,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.658</v>
+        <v>0.664</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>PreCheck - IX precheck denied for Anchor site stating that the BH is not ready</t>
+          <t>IX precheck denied for Anchor site stating that the BH is not ready</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Reporting - during UA engineer shared all techs as new techs incorrectly. RTT from IX vendor was also wrong which didnt provide a clear view on which techs were new and which pre-existing</t>
+          <t>during UA engineer shared all techs as new techs incorrectly. RTT from IX vendor was also wrong which didnt provide a clear view on which techs were new and which pre-existing</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.64</v>
+        <v>0.512</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>32%</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1623,21 +1623,21 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PostCheck - Engineer forgets to paste the manual logs during the post check as there were no logs populated from sim module. Also, site was not unnested from the nest tool after check-out</t>
+          <t>Engineer forgets to paste the manual logs during the post check as there were no logs populated from sim module. Also, site was not unnested from the nest tool after check-out</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Validation &amp; QA</t>
+          <t>Documentation &amp; Reporting</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Missing Logs</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.637</v>
+        <v>0.623</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Alarm monitoring - RET naming issue on Alpha Midband naming having an extra '2' with site ID.</t>
+          <t>RET naming issue on Alpha Midband naming having an extra '2' with site ID.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>KPI Monitoring - NR600 cells on the site were locked and showing zero traffic. This degradation was not detected during the general degradation analysis</t>
+          <t>NR600 cells on the site were locked and showing zero traffic. This degradation was not detected during the general degradation analysis</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KPI Monitoring - NR600 cells on the site were locked and showing zero traffic. This degradation was not detected during the general degradation analysis</t>
+          <t>NR600 cells on the site were locked and showing zero traffic. This degradation was not detected during the general degradation analysis</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1851,7 +1851,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Other - Engineer missed to unlock the cells in M node during Live operation request..</t>
+          <t>Engineer missed to unlock the cells in M node during Live operation request..</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>PostCheck - Engineer Miss to check Cell Status Verification during POST from OSS as Cells were in Unsync state.</t>
+          <t>Engineer Miss to check Cell Status Verification during POST from OSS as Cells were in Unsync state.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.642</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1936,12 +1936,12 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟢 Low (&lt;30%)</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Implementation - Engineers inadvertently removed I from RET naming when working on 2 sites at same time in the background.</t>
+          <t>Engineers inadvertently removed I from RET naming when working on 2 sites at same time in the background.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nesting - We identified Engineer missed to Nest the site as SA based on the market guideline.</t>
+          <t>We identified Engineer missed to Nest the site as SA based on the market guideline.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Reporting - engineer mistakenly placed a different site id in the subject line. that was a human error (he missed to change the site id when he copy pasted the subject line from a previous UL RSSI TS email</t>
+          <t>engineer mistakenly placed a different site id in the subject line. that was a human error (he missed to change the site id when he copy pasted the subject line from a previous UL RSSI TS email</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PostCheck - Engineer Miss to capture new RSSI imbalance on L21 Gamma</t>
+          <t>Engineer Miss to capture new RSSI imbalance on L21 Gamma</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2150,7 +2150,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>PostCheck - Post check alarms captured but not escalated.</t>
+          <t>Post check alarms captured but not escalated.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2207,7 +2207,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.624</v>
+        <v>0.496</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2221,12 +2221,12 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟢 Low (&lt;30%)</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PostCheck - engineer missed to create fiber issue which was active duirng postcheck.</t>
+          <t>engineer missed to create fiber issue which was active duirng postcheck.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2283,7 +2283,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Implementation - During Alarm monitoring PAG found RET Naming swap between Beta &amp; Gamma controlling unit,</t>
+          <t>During Alarm monitoring PAG found RET Naming swap between Beta &amp; Gamma controlling unit,</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2340,7 +2340,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2364,7 +2364,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Alarm monitoring - Engineer did not identified the SFP issue during Alarm monitoring and in summary table it mentioned as No SFP issues. Also missed to attach the detailed site view snapshot.</t>
+          <t>Engineer did not identified the SFP issue during Alarm monitoring and in summary table it mentioned as No SFP issues. Also missed to attach the detailed site view snapshot.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2387,17 +2387,17 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟢 Low (&lt;30%)</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>PostCheck - During post check, issue escalated to different vendor distro, which is raised by client to correct the distro list.</t>
+          <t>During post check, issue escalated to different vendor distro, which is raised by client to correct the distro list.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>KPI Monitoring - A different set of KPIs was analyzed and reported for degradation, which is not aligned with the agreed process</t>
+          <t>A different set of KPIs was analyzed and reported for degradation, which is not aligned with the agreed process</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.639</v>
+        <v>0.554</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2511,7 +2511,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Nesting - PAG engineer Nested the Site NSA which is not allowed in this Market.</t>
+          <t>PAG engineer Nested the Site NSA which is not allowed in this Market.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Nesting - PAG engineer extended the nest as nSA despite the fact it is not allowed in this market. only SA is allowed.</t>
+          <t>PAG engineer extended the nest as nSA despite the fact it is not allowed in this market. only SA is allowed.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>KPI Monitoring - A different set of KPIs was analyzed and reported for degradation, which is not aligned with the agreed process</t>
+          <t>A different set of KPIs was analyzed and reported for degradation, which is not aligned with the agreed process</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2663,7 +2663,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.639</v>
+        <v>0.554</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2682,7 +2682,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Parameter Baselines - NR UL traffic volume reduction &amp; being shifted to LTE UL traffic post site modification.</t>
+          <t>NR UL traffic volume reduction &amp; being shifted to LTE UL traffic post site modification.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2720,7 +2720,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.597</v>
+        <v>0.603</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2763,7 +2763,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Alarm monitoring - Detailed site view snap in the report wrongly attached from another site .</t>
+          <t>Detailed site view snap in the report wrongly attached from another site .</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2791,12 +2791,12 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟢 Low (&lt;30%)</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2820,7 +2820,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Nesting - AAV site nest extended during Follow Up</t>
+          <t>AAV site nest extended during Follow Up</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Parameter Changes - RET found Max for all the cells during 2 hour alarm monitoring.</t>
+          <t>RET found Max for all the cells during 2 hour alarm monitoring.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2891,7 +2891,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.608</v>
+        <v>0.578</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>PreCheck - IX precheck denied with wrong BH validation from MB. BH was already actualized , but engineer denied IX- precheck with comment BH not actualized</t>
+          <t>IX precheck denied with wrong BH validation from MB. BH was already actualized , but engineer denied IX- precheck with comment BH not actualized</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PostCheck - During post check, issue escalated to different vendor distro, which is raised by client to correct the distro list.</t>
+          <t>During post check, issue escalated to different vendor distro, which is raised by client to correct the distro list.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3024,7 +3024,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Port Matrix - Integration team shared the integration update email with wrong RET naming on Gamma sector for all techs. according port matrix it should be IL11609A_C12JBL and IL11609A_C11KED but they named them IL11609A_C22JBL and IL11609A_C21KED wrongly</t>
+          <t>Integration team shared the integration update email with wrong RET naming on Gamma sector for all techs. according port matrix it should be IL11609A_C12JBL and IL11609A_C11KED but they named them IL11609A_C22JBL and IL11609A_C21KED wrongly</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Nesting - Appalachian Market site nested as NSI from SI nesting during Nest extension leading to Down cell getting nested as NSI</t>
+          <t>Appalachian Market site nested as NSI from SI nesting during Nest extension leading to Down cell getting nested as NSI</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Nesting - Appalachian market site nested as NSI from SI during nest extension</t>
+          <t>Appalachian market site nested as NSI from SI during nest extension</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3219,7 +3219,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Other - PAG ticket moved to Post check without Riot lemming validation</t>
+          <t>PAG ticket moved to Post check without Riot lemming validation</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Other - VONR was not activated despite requested by GC over adhoc and only NRPCI was shared, which was later caught by MS2 team</t>
+          <t>VONR was not activated despite requested by GC over adhoc and only NRPCI was shared, which was later caught by MS2 team</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3290,7 +3290,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.628</v>
+        <v>0.584</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Other - Extreme congestion, low Throughput, AFR, DCR degraded, HSI low speed complaint after site replacement On-Air</t>
+          <t>Extreme congestion, low Throughput, AFR, DCR degraded, HSI low speed complaint after site replacement On-Air</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3347,7 +3347,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.545</v>
+        <v>0.542</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>11%</t>
+          <t>18%</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -3390,21 +3390,21 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Alarm monitoring - During 2 hours alarm monitoring PAG found External alarm 8 : AC SURGE SUPPRESSOR naming is incorrect. This naming should corrected as AC SURGE SUPPRESSOR Fail</t>
+          <t>During 2 hours alarm monitoring PAG found External alarm 8 : AC SURGE SUPPRESSOR naming is incorrect. This naming should corrected as AC SURGE SUPPRESSOR Fail</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Documentation &amp; Reporting</t>
+          <t>Configuration &amp; Data Mismatch</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>RET Naming</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.679</v>
+        <v>0.65</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -3423,7 +3423,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Reporting - In the Unlock announcement email, the engineer marked VSWR as Fail and RSSI as Pass. However, on site the actual status is VSWR Pass and RSSI Fail. This discrepancy is providing incorrect information to the market &amp; Ericsson IX team for troubleshooting the issue.</t>
+          <t>In the Unlock announcement email, the engineer marked VSWR as Fail and RSSI as Pass. However, on site the actual status is VSWR Pass and RSSI Fail. This discrepancy is providing incorrect information to the market &amp; Ericsson IX team for troubleshooting the issue.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3461,7 +3461,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.606</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -3480,7 +3480,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>RIOT - In-complete lemming snapshot was uploaded inside the ticket while serving the request. GC requested for L7, NR6 ABC but engineer uploaded the Lemming snap for only 2 sectors and Gamma sector was missing..</t>
+          <t>In-complete lemming snapshot was uploaded inside the ticket while serving the request. GC requested for L7, NR6 ABC but engineer uploaded the Lemming snap for only 2 sectors and Gamma sector was missing..</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3561,12 +3561,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>COP - DL TPUT decrease in post Cluster KPI</t>
+          <t>DL TPUT decrease in post Cluster KPI</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Configuration &amp; Data Mismatch</t>
+          <t>Validation &amp; QA</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3575,7 +3575,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.627</v>
+        <v>0.639</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>11%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Other - SC06651A Mobility and DCR starts to deviate when SC70149A (MS2 site) was on-aired</t>
+          <t>SC06651A Mobility and DCR starts to deviate when SC70149A (MS2 site) was on-aired</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.651</v>
+        <v>0.588</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>11%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Alarm monitoring - During 2 Hour alarm monitoring Low band and Mid band RET naming was swapped for Alpha &amp; Beta.</t>
+          <t>During 2 Hour alarm monitoring Low band and Mid band RET naming was swapped for Alpha &amp; Beta.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -3732,7 +3732,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>PostCheck - RET issue were missed to report in Post check</t>
+          <t>RET issue were missed to report in Post check</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3765,7 +3765,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>PostCheck - Post check Miss- RSSI on L21 was not created and escalated</t>
+          <t>Post check Miss- RSSI on L21 was not created and escalated</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3803,7 +3803,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0.75</v>
+        <v>0.724</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Alarm monitoring - During 2 hours alarm monitoring PAG found different site id in RET naming for low band ( Snapshot has been attached on RCA upload section).</t>
+          <t>During 2 hours alarm monitoring PAG found different site id in RET naming for low band ( Snapshot has been attached on RCA upload section).</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Lemming - NR25_2C_NR19_2C Gamma lemming snap is not uploaded in FCI while serving GC request.</t>
+          <t>NR25_2C_NR19_2C Gamma lemming snap is not uploaded in FCI while serving GC request.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3917,7 +3917,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>0.639</v>
+        <v>0.607</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -4050,7 +4050,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -4107,7 +4107,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -4221,7 +4221,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -4449,7 +4449,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
@@ -4506,7 +4506,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -4848,7 +4848,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -5076,7 +5076,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -5304,7 +5304,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -5475,7 +5475,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
@@ -5646,7 +5646,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -6330,7 +6330,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -6387,7 +6387,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -6444,7 +6444,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -6615,7 +6615,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -6843,7 +6843,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
@@ -7128,7 +7128,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J112" t="inlineStr">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J117" t="inlineStr">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -7869,7 +7869,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J125" t="inlineStr">
@@ -7983,7 +7983,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J127" t="inlineStr">
@@ -8040,7 +8040,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
@@ -8097,7 +8097,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
@@ -8154,7 +8154,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J131" t="inlineStr">
@@ -8439,7 +8439,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
@@ -8667,7 +8667,7 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J139" t="inlineStr">
@@ -8724,7 +8724,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J140" t="inlineStr">
@@ -8895,7 +8895,7 @@
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -9066,7 +9066,7 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J146" t="inlineStr">
@@ -9408,7 +9408,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
@@ -9465,7 +9465,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
@@ -9579,7 +9579,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J155" t="inlineStr">
@@ -9636,7 +9636,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
@@ -9750,7 +9750,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
@@ -9978,7 +9978,7 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
@@ -10035,7 +10035,7 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
@@ -10206,7 +10206,7 @@
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J166" t="inlineStr">
@@ -10548,7 +10548,7 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J172" t="inlineStr">
@@ -10605,7 +10605,7 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J173" t="inlineStr">
@@ -10662,7 +10662,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
@@ -10833,7 +10833,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
@@ -10890,7 +10890,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
@@ -10947,7 +10947,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
@@ -11004,7 +11004,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
@@ -11061,7 +11061,7 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J181" t="inlineStr">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
@@ -11175,7 +11175,7 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
@@ -11232,7 +11232,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
@@ -11289,7 +11289,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>29%</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -11802,7 +11802,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>22%</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
@@ -11859,7 +11859,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
@@ -11973,7 +11973,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>31%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J201" t="inlineStr">
@@ -12600,7 +12600,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J208" t="inlineStr">
@@ -12657,7 +12657,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J209" t="inlineStr">
@@ -12714,7 +12714,7 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J210" t="inlineStr">
@@ -12771,7 +12771,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J211" t="inlineStr">
@@ -12828,7 +12828,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J212" t="inlineStr">
@@ -12942,7 +12942,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>14%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J214" t="inlineStr">
@@ -13854,7 +13854,7 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J230" t="inlineStr">
@@ -14880,7 +14880,7 @@
       </c>
       <c r="I248" t="inlineStr">
         <is>
-          <t>22%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J248" t="inlineStr">
@@ -15108,7 +15108,7 @@
       </c>
       <c r="I252" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J252" t="inlineStr">
@@ -15279,7 +15279,7 @@
       </c>
       <c r="I255" t="inlineStr">
         <is>
-          <t>19%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="J255" t="inlineStr">
@@ -15336,7 +15336,7 @@
       </c>
       <c r="I256" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J256" t="inlineStr">
@@ -15393,7 +15393,7 @@
       </c>
       <c r="I257" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J257" t="inlineStr">
@@ -15450,7 +15450,7 @@
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J258" t="inlineStr">
@@ -15507,7 +15507,7 @@
       </c>
       <c r="I259" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J259" t="inlineStr">
@@ -15621,7 +15621,7 @@
       </c>
       <c r="I261" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J261" t="inlineStr">
@@ -15678,7 +15678,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>14%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
@@ -15792,7 +15792,7 @@
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J264" t="inlineStr">
@@ -15849,7 +15849,7 @@
       </c>
       <c r="I265" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J265" t="inlineStr">
@@ -15906,7 +15906,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J266" t="inlineStr">
@@ -16020,7 +16020,7 @@
       </c>
       <c r="I268" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J268" t="inlineStr">
@@ -16362,7 +16362,7 @@
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J274" t="inlineStr">
@@ -16476,7 +16476,7 @@
       </c>
       <c r="I276" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J276" t="inlineStr">
@@ -16533,7 +16533,7 @@
       </c>
       <c r="I277" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J277" t="inlineStr">
@@ -16590,7 +16590,7 @@
       </c>
       <c r="I278" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J278" t="inlineStr">
@@ -16647,7 +16647,7 @@
       </c>
       <c r="I279" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J279" t="inlineStr">
@@ -16704,7 +16704,7 @@
       </c>
       <c r="I280" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="J280" t="inlineStr">
@@ -16761,7 +16761,7 @@
       </c>
       <c r="I281" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J281" t="inlineStr">
@@ -16818,7 +16818,7 @@
       </c>
       <c r="I282" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J282" t="inlineStr">
@@ -16875,7 +16875,7 @@
       </c>
       <c r="I283" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J283" t="inlineStr">
@@ -16989,7 +16989,7 @@
       </c>
       <c r="I285" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J285" t="inlineStr">
@@ -17046,7 +17046,7 @@
       </c>
       <c r="I286" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J286" t="inlineStr">
@@ -17103,7 +17103,7 @@
       </c>
       <c r="I287" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J287" t="inlineStr">
@@ -17160,7 +17160,7 @@
       </c>
       <c r="I288" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J288" t="inlineStr">
@@ -17274,7 +17274,7 @@
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="J290" t="inlineStr">
@@ -17502,7 +17502,7 @@
       </c>
       <c r="I294" t="inlineStr">
         <is>
-          <t>18%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="J294" t="inlineStr">
@@ -17673,7 +17673,7 @@
       </c>
       <c r="I297" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J297" t="inlineStr">
@@ -18015,7 +18015,7 @@
       </c>
       <c r="I303" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="J303" t="inlineStr">
@@ -18072,7 +18072,7 @@
       </c>
       <c r="I304" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J304" t="inlineStr">
@@ -18129,7 +18129,7 @@
       </c>
       <c r="I305" t="inlineStr">
         <is>
-          <t>17%</t>
+          <t>18%</t>
         </is>
       </c>
       <c r="J305" t="inlineStr">
@@ -18186,7 +18186,7 @@
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J306" t="inlineStr">
@@ -18243,7 +18243,7 @@
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J307" t="inlineStr">
@@ -18300,7 +18300,7 @@
       </c>
       <c r="I308" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J308" t="inlineStr">
@@ -18357,7 +18357,7 @@
       </c>
       <c r="I309" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J309" t="inlineStr">
@@ -18414,7 +18414,7 @@
       </c>
       <c r="I310" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J310" t="inlineStr">
@@ -18585,7 +18585,7 @@
       </c>
       <c r="I313" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J313" t="inlineStr">
@@ -18642,7 +18642,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>17%</t>
+          <t>19%</t>
         </is>
       </c>
       <c r="J314" t="inlineStr">
@@ -18813,7 +18813,7 @@
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J317" t="inlineStr">
@@ -18984,7 +18984,7 @@
       </c>
       <c r="I320" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J320" t="inlineStr">
@@ -19041,7 +19041,7 @@
       </c>
       <c r="I321" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J321" t="inlineStr">
@@ -19098,7 +19098,7 @@
       </c>
       <c r="I322" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J322" t="inlineStr">
@@ -19212,7 +19212,7 @@
       </c>
       <c r="I324" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J324" t="inlineStr">
@@ -19326,7 +19326,7 @@
       </c>
       <c r="I326" t="inlineStr">
         <is>
-          <t>19%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J326" t="inlineStr">
@@ -19440,7 +19440,7 @@
       </c>
       <c r="I328" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J328" t="inlineStr">
@@ -19725,7 +19725,7 @@
       </c>
       <c r="I333" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J333" t="inlineStr">
@@ -19782,7 +19782,7 @@
       </c>
       <c r="I334" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="J334" t="inlineStr">
@@ -19839,7 +19839,7 @@
       </c>
       <c r="I335" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>12%</t>
         </is>
       </c>
       <c r="J335" t="inlineStr">
@@ -20238,7 +20238,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>13%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J342" t="inlineStr">
@@ -20295,7 +20295,7 @@
       </c>
       <c r="I343" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J343" t="inlineStr">
@@ -20352,7 +20352,7 @@
       </c>
       <c r="I344" t="inlineStr">
         <is>
-          <t>14%</t>
+          <t>17%</t>
         </is>
       </c>
       <c r="J344" t="inlineStr">
@@ -20409,7 +20409,7 @@
       </c>
       <c r="I345" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>9%</t>
         </is>
       </c>
       <c r="J345" t="inlineStr">
@@ -20580,7 +20580,7 @@
       </c>
       <c r="I348" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J348" t="inlineStr">
@@ -20637,7 +20637,7 @@
       </c>
       <c r="I349" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>15%</t>
         </is>
       </c>
       <c r="J349" t="inlineStr">
@@ -20803,12 +20803,12 @@
       </c>
       <c r="H352" t="inlineStr">
         <is>
-          <t>🟢 Low (&lt;30%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I352" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="J352" t="inlineStr">
@@ -20865,7 +20865,7 @@
       </c>
       <c r="I353" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>11%</t>
         </is>
       </c>
       <c r="J353" t="inlineStr">
@@ -20922,7 +20922,7 @@
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t>11%</t>
+          <t>13%</t>
         </is>
       </c>
       <c r="J354" t="inlineStr">
@@ -21150,7 +21150,7 @@
       </c>
       <c r="I358" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J358" t="inlineStr">
@@ -21321,7 +21321,7 @@
       </c>
       <c r="I361" t="inlineStr">
         <is>
-          <t>11%</t>
+          <t>13%</t>
         </is>
       </c>
       <c r="J361" t="inlineStr">
@@ -21720,7 +21720,7 @@
       </c>
       <c r="I368" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J368" t="inlineStr">
@@ -22005,7 +22005,7 @@
       </c>
       <c r="I373" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J373" t="inlineStr">
@@ -22176,7 +22176,7 @@
       </c>
       <c r="I376" t="inlineStr">
         <is>
-          <t>31%</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="J376" t="inlineStr">
@@ -22233,7 +22233,7 @@
       </c>
       <c r="I377" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J377" t="inlineStr">
@@ -22306,9 +22306,693 @@
       <c r="L378" t="inlineStr"/>
       <c r="M378" t="inlineStr"/>
     </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>377</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Incorrect Port matrix. Alpha has RET marked as TU03190A _A22LB instead of TU03190A_A12JLB.</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>Port Matrix Mismatch</t>
+        </is>
+      </c>
+      <c r="E379" t="n">
+        <v>0.639</v>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>78%</t>
+        </is>
+      </c>
+      <c r="J379" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K379" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L379" t="inlineStr"/>
+      <c r="M379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>378</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>CBN validation snapshot missing in mail body</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Documentation &amp; Reporting</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>Missing Snapshot</t>
+        </is>
+      </c>
+      <c r="E380" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="J380" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K380" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L380" t="inlineStr"/>
+      <c r="M380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>379</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>CBN validation snapshot missing in mail body</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Documentation &amp; Reporting</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>Missing Snapshot</t>
+        </is>
+      </c>
+      <c r="E381" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="J381" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K381" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L381" t="inlineStr"/>
+      <c r="M381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>CBN validation snapshot missing in mail body</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Documentation &amp; Reporting</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>Missing Snapshot</t>
+        </is>
+      </c>
+      <c r="E382" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="J382" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K382" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L382" t="inlineStr"/>
+      <c r="M382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>381</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>E911 completion mail has summary table copied from E911 Go mail</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>Documentation &amp; Reporting</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E383" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>81%</t>
+        </is>
+      </c>
+      <c r="J383" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K383" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L383" t="inlineStr"/>
+      <c r="M383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>382</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>In E911 complete mail's summary table, 4 sectors (ABGD) has been mentioned, despite having 3 sectors (ABG) in actual</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>Documentation &amp; Reporting</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E384" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>85%</t>
+        </is>
+      </c>
+      <c r="J384" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K384" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L384" t="inlineStr"/>
+      <c r="M384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>383</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>PSAP contact info table missing in E911 GO mail</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>Documentation &amp; Reporting</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>Missing Information</t>
+        </is>
+      </c>
+      <c r="E385" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H385" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>96%</t>
+        </is>
+      </c>
+      <c r="J385" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K385" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L385" t="inlineStr"/>
+      <c r="M385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>384</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>E-tilt missing in RFDS Angle-E-Tilt is mentioned only for Delta sectors (both Mid and Low bands) in the proposed RFDS</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>Nesting &amp; Tool Errors</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E386" t="n">
+        <v>0.491</v>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H386" t="inlineStr">
+        <is>
+          <t>🟢 Low (&lt;30%)</t>
+        </is>
+      </c>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="J386" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K386" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L386" t="inlineStr"/>
+      <c r="M386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>385</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Site is having 1x1 (mid cell so it's 1×1 ) per sector RET configuration, but PM is designed 2x2 per sector configuration</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E387" t="n">
+        <v>0.593</v>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H387" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>83%</t>
+        </is>
+      </c>
+      <c r="J387" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K387" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L387" t="inlineStr"/>
+      <c r="M387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>386</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Site has GSM available and RFDS also but in Port Matrix not available GSM</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>Port Matrix Mismatch</t>
+        </is>
+      </c>
+      <c r="E388" t="n">
+        <v>0.694</v>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H388" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>98%</t>
+        </is>
+      </c>
+      <c r="J388" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K388" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L388" t="inlineStr"/>
+      <c r="M388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>387</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Mismatch in RFDS and CIQ. As per RFDS L700 not available on site.but its showing in CIQ &amp; SCF</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>RFDS Mismatch</t>
+        </is>
+      </c>
+      <c r="E389" t="n">
+        <v>0.741</v>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>98%</t>
+        </is>
+      </c>
+      <c r="J389" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K389" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L389" t="inlineStr"/>
+      <c r="M389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>388</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Mismatch in PORT matrix and RET. N2100 technology is included in the RET definition naming as per the port matrix. However, as per the current site configuration, N2100 is not available on Site</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Configuration &amp; Data Mismatch</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>Port Matrix Mismatch</t>
+        </is>
+      </c>
+      <c r="E390" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>Unclassified</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>🔴 High Risk (&gt;70%)</t>
+        </is>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>97%</t>
+        </is>
+      </c>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="K390" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="L390" t="inlineStr"/>
+      <c r="M390" t="inlineStr"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="K2:K378" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K2:K390" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>'Category Reference'!$A$2:$A$100</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update report generator and regenerate report assets
- Update report_generator.py with improvements
- Regenerate SLA charts (aging, waterfall, funnel)
- Regenerate engineer quadrant visualization
- Regenerate executive scorecard
- Update Strategic_Report.xlsx with latest data
- Update classification_feedback.xlsx

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/classification_feedback.xlsx
+++ b/classification_feedback.xlsx
@@ -705,7 +705,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Generated: 2026-02-04 21:08</t>
+          <t>Generated: 2026-02-05 08:53</t>
         </is>
       </c>
     </row>
@@ -1884,7 +1884,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -3024,7 +3024,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -11916,7 +11916,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
@@ -12030,7 +12030,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J198" t="inlineStr">
@@ -15678,7 +15678,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
@@ -18414,7 +18414,7 @@
       </c>
       <c r="I310" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J310" t="inlineStr">
@@ -18813,7 +18813,7 @@
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="J317" t="inlineStr">
@@ -19326,7 +19326,7 @@
       </c>
       <c r="I326" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>32%</t>
         </is>
       </c>
       <c r="J326" t="inlineStr">
@@ -19497,7 +19497,7 @@
       </c>
       <c r="I329" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J329" t="inlineStr">
@@ -19554,7 +19554,7 @@
       </c>
       <c r="I330" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J330" t="inlineStr">
@@ -19611,7 +19611,7 @@
       </c>
       <c r="I331" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J331" t="inlineStr">
@@ -19668,7 +19668,7 @@
       </c>
       <c r="I332" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J332" t="inlineStr">
@@ -20409,7 +20409,7 @@
       </c>
       <c r="I345" t="inlineStr">
         <is>
-          <t>14%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J345" t="inlineStr">
@@ -20523,7 +20523,7 @@
       </c>
       <c r="I347" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J347" t="inlineStr">
@@ -20580,7 +20580,7 @@
       </c>
       <c r="I348" t="inlineStr">
         <is>
-          <t>68%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="J348" t="inlineStr">
@@ -21777,7 +21777,7 @@
       </c>
       <c r="I369" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J369" t="inlineStr">
@@ -21891,7 +21891,7 @@
       </c>
       <c r="I371" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J371" t="inlineStr">
@@ -21948,7 +21948,7 @@
       </c>
       <c r="I372" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J372" t="inlineStr">

</xml_diff>

<commit_message>
Update charts and feedback with corrected financial data
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/classification_feedback.xlsx
+++ b/classification_feedback.xlsx
@@ -705,7 +705,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Generated: 2026-02-05 23:35</t>
+          <t>Generated: 2026-02-06 00:55</t>
         </is>
       </c>
     </row>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -13284,7 +13284,7 @@
       </c>
       <c r="I220" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J220" t="inlineStr">
@@ -19098,7 +19098,7 @@
       </c>
       <c r="I322" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J322" t="inlineStr">
@@ -19326,7 +19326,7 @@
       </c>
       <c r="I326" t="inlineStr">
         <is>
-          <t>32%</t>
+          <t>31%</t>
         </is>
       </c>
       <c r="J326" t="inlineStr">
@@ -19611,7 +19611,7 @@
       </c>
       <c r="I331" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J331" t="inlineStr">
@@ -20238,7 +20238,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J342" t="inlineStr">
@@ -20865,7 +20865,7 @@
       </c>
       <c r="I353" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="J353" t="inlineStr">

</xml_diff>

<commit_message>
Consolidate price catalog as single source of truth, update charts
Refactor dashboard to delegate all pricing logic to the PriceCatalog class
instead of duplicating loading/calculation code. Update financial metrics,
scoring, and regenerate charts with corrected cost data.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/classification_feedback.xlsx
+++ b/classification_feedback.xlsx
@@ -705,7 +705,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Generated: 2026-02-06 00:55</t>
+          <t>Generated: 2026-02-09 10:46</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -915,7 +915,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>36%</t>
+          <t>32%</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>18%</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2055,7 +2055,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2283,7 +2283,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2340,7 +2340,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3024,7 +3024,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3247,12 +3247,12 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>🟡 Moderate (30-50%)</t>
+          <t>🟢 Low (&lt;30%)</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>37%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>13%</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -3423,7 +3423,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3480,7 +3480,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>11%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>12%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -3765,7 +3765,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -4050,7 +4050,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -4107,7 +4107,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -4221,7 +4221,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -4449,7 +4449,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
@@ -4506,7 +4506,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -4677,7 +4677,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -4734,7 +4734,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -4791,7 +4791,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
@@ -4905,7 +4905,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -5076,7 +5076,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -5133,7 +5133,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
@@ -5190,7 +5190,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
@@ -5247,7 +5247,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
@@ -5304,7 +5304,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -5361,7 +5361,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -5475,7 +5475,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
@@ -5532,7 +5532,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
@@ -5646,7 +5646,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -5760,7 +5760,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
@@ -5817,7 +5817,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
@@ -5931,7 +5931,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
@@ -6045,7 +6045,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -6216,7 +6216,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -6330,7 +6330,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -6387,7 +6387,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -6444,7 +6444,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -6558,7 +6558,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
@@ -6615,7 +6615,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
@@ -6672,7 +6672,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
@@ -6729,7 +6729,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -6843,7 +6843,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
@@ -6900,7 +6900,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
@@ -6957,7 +6957,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
@@ -7014,7 +7014,7 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
@@ -7071,7 +7071,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
@@ -7128,7 +7128,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J112" t="inlineStr">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J113" t="inlineStr">
@@ -7242,7 +7242,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
@@ -7299,7 +7299,7 @@
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J115" t="inlineStr">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
@@ -7527,7 +7527,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J119" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -7641,7 +7641,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J121" t="inlineStr">
@@ -7698,7 +7698,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J122" t="inlineStr">
@@ -7755,7 +7755,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -7812,7 +7812,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -7869,7 +7869,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J125" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
@@ -7983,7 +7983,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J127" t="inlineStr">
@@ -8040,7 +8040,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
@@ -8097,7 +8097,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
@@ -8154,7 +8154,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J131" t="inlineStr">
@@ -8268,7 +8268,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J132" t="inlineStr">
@@ -8325,7 +8325,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J133" t="inlineStr">
@@ -8382,7 +8382,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J134" t="inlineStr">
@@ -8439,7 +8439,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
@@ -8496,7 +8496,7 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J136" t="inlineStr">
@@ -8553,7 +8553,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J137" t="inlineStr">
@@ -8610,7 +8610,7 @@
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J138" t="inlineStr">
@@ -8667,7 +8667,7 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="J139" t="inlineStr">
@@ -8724,7 +8724,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J140" t="inlineStr">
@@ -8781,7 +8781,7 @@
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J141" t="inlineStr">
@@ -8895,7 +8895,7 @@
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -8952,7 +8952,7 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
@@ -9009,7 +9009,7 @@
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J145" t="inlineStr">
@@ -9066,7 +9066,7 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J146" t="inlineStr">
@@ -9123,7 +9123,7 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J147" t="inlineStr">
@@ -9180,7 +9180,7 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J148" t="inlineStr">
@@ -9237,7 +9237,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J149" t="inlineStr">
@@ -9294,7 +9294,7 @@
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J150" t="inlineStr">
@@ -9351,7 +9351,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J151" t="inlineStr">
@@ -9408,7 +9408,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
@@ -9465,7 +9465,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
@@ -9522,7 +9522,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J154" t="inlineStr">
@@ -9579,7 +9579,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J155" t="inlineStr">
@@ -9636,7 +9636,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
@@ -9693,7 +9693,7 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
@@ -9750,7 +9750,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>36%</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
@@ -9807,7 +9807,7 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
@@ -10035,7 +10035,7 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
@@ -10092,7 +10092,7 @@
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
@@ -10149,7 +10149,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
@@ -10263,7 +10263,7 @@
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J167" t="inlineStr">
@@ -10320,7 +10320,7 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
@@ -10377,7 +10377,7 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
@@ -10434,7 +10434,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
@@ -10548,7 +10548,7 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J172" t="inlineStr">
@@ -10605,7 +10605,7 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J173" t="inlineStr">
@@ -10662,7 +10662,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
@@ -10719,7 +10719,7 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J175" t="inlineStr">
@@ -10776,7 +10776,7 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J176" t="inlineStr">
@@ -10833,7 +10833,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
@@ -10890,7 +10890,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
@@ -10947,7 +10947,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
@@ -11004,7 +11004,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
@@ -11175,7 +11175,7 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
@@ -11232,7 +11232,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
@@ -11289,7 +11289,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
@@ -11346,7 +11346,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
@@ -11460,7 +11460,7 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
@@ -11517,7 +11517,7 @@
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J189" t="inlineStr">
@@ -11574,7 +11574,7 @@
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J190" t="inlineStr">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -11688,7 +11688,7 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J192" t="inlineStr">
@@ -11745,7 +11745,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
@@ -11802,7 +11802,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
@@ -11859,7 +11859,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
@@ -11916,7 +11916,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
@@ -11973,7 +11973,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
@@ -12030,7 +12030,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J198" t="inlineStr">
@@ -12144,7 +12144,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J200" t="inlineStr">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J201" t="inlineStr">
@@ -12258,7 +12258,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J202" t="inlineStr">
@@ -12315,7 +12315,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J203" t="inlineStr">
@@ -12372,7 +12372,7 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J204" t="inlineStr">
@@ -12429,7 +12429,7 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J205" t="inlineStr">
@@ -12486,7 +12486,7 @@
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J206" t="inlineStr">
@@ -12543,7 +12543,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J207" t="inlineStr">
@@ -12600,7 +12600,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J208" t="inlineStr">
@@ -12657,7 +12657,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J209" t="inlineStr">
@@ -12771,7 +12771,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="J211" t="inlineStr">
@@ -12828,7 +12828,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>38%</t>
         </is>
       </c>
       <c r="J212" t="inlineStr">
@@ -12885,7 +12885,7 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J213" t="inlineStr">
@@ -12942,7 +12942,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>22%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J214" t="inlineStr">
@@ -12999,7 +12999,7 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J215" t="inlineStr">
@@ -13170,7 +13170,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J218" t="inlineStr">
@@ -13227,7 +13227,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J219" t="inlineStr">
@@ -13284,7 +13284,7 @@
       </c>
       <c r="I220" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J220" t="inlineStr">
@@ -13341,7 +13341,7 @@
       </c>
       <c r="I221" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J221" t="inlineStr">
@@ -13398,7 +13398,7 @@
       </c>
       <c r="I222" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J222" t="inlineStr">
@@ -13455,7 +13455,7 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J223" t="inlineStr">
@@ -13512,7 +13512,7 @@
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J224" t="inlineStr">
@@ -13569,7 +13569,7 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J225" t="inlineStr">
@@ -13626,7 +13626,7 @@
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J226" t="inlineStr">
@@ -13740,7 +13740,7 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J228" t="inlineStr">
@@ -13797,7 +13797,7 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J229" t="inlineStr">
@@ -13854,7 +13854,7 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="J230" t="inlineStr">
@@ -13911,7 +13911,7 @@
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J231" t="inlineStr">
@@ -13968,7 +13968,7 @@
       </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J232" t="inlineStr">
@@ -14025,7 +14025,7 @@
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J233" t="inlineStr">
@@ -14082,7 +14082,7 @@
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J234" t="inlineStr">
@@ -14139,7 +14139,7 @@
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J235" t="inlineStr">
@@ -14196,7 +14196,7 @@
       </c>
       <c r="I236" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J236" t="inlineStr">
@@ -14253,7 +14253,7 @@
       </c>
       <c r="I237" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J237" t="inlineStr">
@@ -14310,7 +14310,7 @@
       </c>
       <c r="I238" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J238" t="inlineStr">
@@ -14367,7 +14367,7 @@
       </c>
       <c r="I239" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J239" t="inlineStr">
@@ -14424,7 +14424,7 @@
       </c>
       <c r="I240" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J240" t="inlineStr">
@@ -14481,7 +14481,7 @@
       </c>
       <c r="I241" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J241" t="inlineStr">
@@ -14538,7 +14538,7 @@
       </c>
       <c r="I242" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J242" t="inlineStr">
@@ -14595,7 +14595,7 @@
       </c>
       <c r="I243" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J243" t="inlineStr">
@@ -14652,7 +14652,7 @@
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J244" t="inlineStr">
@@ -14709,7 +14709,7 @@
       </c>
       <c r="I245" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J245" t="inlineStr">
@@ -14766,7 +14766,7 @@
       </c>
       <c r="I246" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J246" t="inlineStr">
@@ -14823,7 +14823,7 @@
       </c>
       <c r="I247" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J247" t="inlineStr">
@@ -14880,7 +14880,7 @@
       </c>
       <c r="I248" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="J248" t="inlineStr">
@@ -14994,7 +14994,7 @@
       </c>
       <c r="I250" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J250" t="inlineStr">
@@ -15165,7 +15165,7 @@
       </c>
       <c r="I253" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J253" t="inlineStr">
@@ -15222,7 +15222,7 @@
       </c>
       <c r="I254" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J254" t="inlineStr">
@@ -15336,7 +15336,7 @@
       </c>
       <c r="I256" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J256" t="inlineStr">
@@ -15393,7 +15393,7 @@
       </c>
       <c r="I257" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J257" t="inlineStr">
@@ -15450,7 +15450,7 @@
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J258" t="inlineStr">
@@ -15507,7 +15507,7 @@
       </c>
       <c r="I259" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J259" t="inlineStr">
@@ -15564,7 +15564,7 @@
       </c>
       <c r="I260" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J260" t="inlineStr">
@@ -15621,7 +15621,7 @@
       </c>
       <c r="I261" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J261" t="inlineStr">
@@ -15678,7 +15678,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
@@ -15735,7 +15735,7 @@
       </c>
       <c r="I263" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="J263" t="inlineStr">
@@ -15792,7 +15792,7 @@
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J264" t="inlineStr">
@@ -15906,7 +15906,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J266" t="inlineStr">
@@ -16077,7 +16077,7 @@
       </c>
       <c r="I269" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J269" t="inlineStr">
@@ -16134,7 +16134,7 @@
       </c>
       <c r="I270" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J270" t="inlineStr">
@@ -16191,7 +16191,7 @@
       </c>
       <c r="I271" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J271" t="inlineStr">
@@ -16248,7 +16248,7 @@
       </c>
       <c r="I272" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J272" t="inlineStr">
@@ -16305,7 +16305,7 @@
       </c>
       <c r="I273" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J273" t="inlineStr">
@@ -16362,7 +16362,7 @@
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J274" t="inlineStr">
@@ -16419,7 +16419,7 @@
       </c>
       <c r="I275" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J275" t="inlineStr">
@@ -16476,7 +16476,7 @@
       </c>
       <c r="I276" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J276" t="inlineStr">
@@ -16590,7 +16590,7 @@
       </c>
       <c r="I278" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J278" t="inlineStr">
@@ -16704,7 +16704,7 @@
       </c>
       <c r="I280" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="J280" t="inlineStr">
@@ -16932,7 +16932,7 @@
       </c>
       <c r="I284" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J284" t="inlineStr">
@@ -17103,7 +17103,7 @@
       </c>
       <c r="I287" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J287" t="inlineStr">
@@ -17160,7 +17160,7 @@
       </c>
       <c r="I288" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J288" t="inlineStr">
@@ -17217,7 +17217,7 @@
       </c>
       <c r="I289" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J289" t="inlineStr">
@@ -17274,7 +17274,7 @@
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="J290" t="inlineStr">
@@ -17331,7 +17331,7 @@
       </c>
       <c r="I291" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J291" t="inlineStr">
@@ -17388,7 +17388,7 @@
       </c>
       <c r="I292" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J292" t="inlineStr">
@@ -17445,7 +17445,7 @@
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J293" t="inlineStr">
@@ -17502,7 +17502,7 @@
       </c>
       <c r="I294" t="inlineStr">
         <is>
-          <t>37%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="J294" t="inlineStr">
@@ -17616,7 +17616,7 @@
       </c>
       <c r="I296" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J296" t="inlineStr">
@@ -17673,7 +17673,7 @@
       </c>
       <c r="I297" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J297" t="inlineStr">
@@ -17730,7 +17730,7 @@
       </c>
       <c r="I298" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J298" t="inlineStr">
@@ -17787,7 +17787,7 @@
       </c>
       <c r="I299" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J299" t="inlineStr">
@@ -17844,7 +17844,7 @@
       </c>
       <c r="I300" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J300" t="inlineStr">
@@ -17901,7 +17901,7 @@
       </c>
       <c r="I301" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J301" t="inlineStr">
@@ -17958,7 +17958,7 @@
       </c>
       <c r="I302" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J302" t="inlineStr">
@@ -18015,7 +18015,7 @@
       </c>
       <c r="I303" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="J303" t="inlineStr">
@@ -18072,7 +18072,7 @@
       </c>
       <c r="I304" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J304" t="inlineStr">
@@ -18129,7 +18129,7 @@
       </c>
       <c r="I305" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="J305" t="inlineStr">
@@ -18186,7 +18186,7 @@
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J306" t="inlineStr">
@@ -18243,7 +18243,7 @@
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J307" t="inlineStr">
@@ -18300,7 +18300,7 @@
       </c>
       <c r="I308" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J308" t="inlineStr">
@@ -18357,7 +18357,7 @@
       </c>
       <c r="I309" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J309" t="inlineStr">
@@ -18414,7 +18414,7 @@
       </c>
       <c r="I310" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="J310" t="inlineStr">
@@ -18471,7 +18471,7 @@
       </c>
       <c r="I311" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J311" t="inlineStr">
@@ -18528,7 +18528,7 @@
       </c>
       <c r="I312" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J312" t="inlineStr">
@@ -18585,7 +18585,7 @@
       </c>
       <c r="I313" t="inlineStr">
         <is>
-          <t>27%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J313" t="inlineStr">
@@ -18642,7 +18642,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J314" t="inlineStr">
@@ -18699,7 +18699,7 @@
       </c>
       <c r="I315" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J315" t="inlineStr">
@@ -18756,7 +18756,7 @@
       </c>
       <c r="I316" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J316" t="inlineStr">
@@ -18927,7 +18927,7 @@
       </c>
       <c r="I319" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J319" t="inlineStr">
@@ -19041,7 +19041,7 @@
       </c>
       <c r="I321" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J321" t="inlineStr">
@@ -19098,7 +19098,7 @@
       </c>
       <c r="I322" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J322" t="inlineStr">
@@ -19155,7 +19155,7 @@
       </c>
       <c r="I323" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J323" t="inlineStr">
@@ -19212,7 +19212,7 @@
       </c>
       <c r="I324" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J324" t="inlineStr">
@@ -19269,7 +19269,7 @@
       </c>
       <c r="I325" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J325" t="inlineStr">
@@ -19321,12 +19321,12 @@
       </c>
       <c r="H326" t="inlineStr">
         <is>
-          <t>🟡 Moderate (30-50%)</t>
+          <t>🟢 Low (&lt;30%)</t>
         </is>
       </c>
       <c r="I326" t="inlineStr">
         <is>
-          <t>31%</t>
+          <t>29%</t>
         </is>
       </c>
       <c r="J326" t="inlineStr">
@@ -19383,7 +19383,7 @@
       </c>
       <c r="I327" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="J327" t="inlineStr">
@@ -19440,7 +19440,7 @@
       </c>
       <c r="I328" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J328" t="inlineStr">
@@ -19497,7 +19497,7 @@
       </c>
       <c r="I329" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J329" t="inlineStr">
@@ -19554,7 +19554,7 @@
       </c>
       <c r="I330" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J330" t="inlineStr">
@@ -19611,7 +19611,7 @@
       </c>
       <c r="I331" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J331" t="inlineStr">
@@ -19668,7 +19668,7 @@
       </c>
       <c r="I332" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J332" t="inlineStr">
@@ -19725,7 +19725,7 @@
       </c>
       <c r="I333" t="inlineStr">
         <is>
-          <t>29%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="J333" t="inlineStr">
@@ -19777,12 +19777,12 @@
       </c>
       <c r="H334" t="inlineStr">
         <is>
-          <t>🟠 Elevated (50-70%)</t>
+          <t>🔴 High Risk (&gt;70%)</t>
         </is>
       </c>
       <c r="I334" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="J334" t="inlineStr">
@@ -19834,12 +19834,12 @@
       </c>
       <c r="H335" t="inlineStr">
         <is>
-          <t>🟠 Elevated (50-70%)</t>
+          <t>🔴 High Risk (&gt;70%)</t>
         </is>
       </c>
       <c r="I335" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>71%</t>
         </is>
       </c>
       <c r="J335" t="inlineStr">
@@ -19896,7 +19896,7 @@
       </c>
       <c r="I336" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J336" t="inlineStr">
@@ -19953,7 +19953,7 @@
       </c>
       <c r="I337" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J337" t="inlineStr">
@@ -20010,7 +20010,7 @@
       </c>
       <c r="I338" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J338" t="inlineStr">
@@ -20067,7 +20067,7 @@
       </c>
       <c r="I339" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J339" t="inlineStr">
@@ -20124,7 +20124,7 @@
       </c>
       <c r="I340" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J340" t="inlineStr">
@@ -20181,7 +20181,7 @@
       </c>
       <c r="I341" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J341" t="inlineStr">
@@ -20238,7 +20238,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J342" t="inlineStr">
@@ -20295,7 +20295,7 @@
       </c>
       <c r="I343" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J343" t="inlineStr">
@@ -20352,7 +20352,7 @@
       </c>
       <c r="I344" t="inlineStr">
         <is>
-          <t>17%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J344" t="inlineStr">
@@ -20409,7 +20409,7 @@
       </c>
       <c r="I345" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>10%</t>
         </is>
       </c>
       <c r="J345" t="inlineStr">
@@ -20466,7 +20466,7 @@
       </c>
       <c r="I346" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J346" t="inlineStr">
@@ -20523,7 +20523,7 @@
       </c>
       <c r="I347" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J347" t="inlineStr">
@@ -20575,7 +20575,7 @@
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>🟠 Elevated (50-70%)</t>
+          <t>🔴 High Risk (&gt;70%)</t>
         </is>
       </c>
       <c r="I348" t="inlineStr">
@@ -20637,7 +20637,7 @@
       </c>
       <c r="I349" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>29%</t>
         </is>
       </c>
       <c r="J349" t="inlineStr">
@@ -20694,7 +20694,7 @@
       </c>
       <c r="I350" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J350" t="inlineStr">
@@ -20751,7 +20751,7 @@
       </c>
       <c r="I351" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J351" t="inlineStr">
@@ -20808,7 +20808,7 @@
       </c>
       <c r="I352" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J352" t="inlineStr">
@@ -20917,12 +20917,12 @@
       </c>
       <c r="H354" t="inlineStr">
         <is>
-          <t>🟡 Moderate (30-50%)</t>
+          <t>🟢 Low (&lt;30%)</t>
         </is>
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t>32%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J354" t="inlineStr">
@@ -20979,7 +20979,7 @@
       </c>
       <c r="I355" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>22%</t>
         </is>
       </c>
       <c r="J355" t="inlineStr">
@@ -21036,7 +21036,7 @@
       </c>
       <c r="I356" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J356" t="inlineStr">
@@ -21093,7 +21093,7 @@
       </c>
       <c r="I357" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J357" t="inlineStr">
@@ -21150,7 +21150,7 @@
       </c>
       <c r="I358" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J358" t="inlineStr">
@@ -21207,7 +21207,7 @@
       </c>
       <c r="I359" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J359" t="inlineStr">
@@ -21264,7 +21264,7 @@
       </c>
       <c r="I360" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J360" t="inlineStr">
@@ -21321,7 +21321,7 @@
       </c>
       <c r="I361" t="inlineStr">
         <is>
-          <t>27%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="J361" t="inlineStr">
@@ -21378,7 +21378,7 @@
       </c>
       <c r="I362" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J362" t="inlineStr">
@@ -21435,7 +21435,7 @@
       </c>
       <c r="I363" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J363" t="inlineStr">
@@ -21492,7 +21492,7 @@
       </c>
       <c r="I364" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J364" t="inlineStr">
@@ -21549,7 +21549,7 @@
       </c>
       <c r="I365" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J365" t="inlineStr">
@@ -21606,7 +21606,7 @@
       </c>
       <c r="I366" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J366" t="inlineStr">
@@ -21663,7 +21663,7 @@
       </c>
       <c r="I367" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J367" t="inlineStr">
@@ -21720,7 +21720,7 @@
       </c>
       <c r="I368" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="J368" t="inlineStr">
@@ -21777,7 +21777,7 @@
       </c>
       <c r="I369" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J369" t="inlineStr">
@@ -21834,7 +21834,7 @@
       </c>
       <c r="I370" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J370" t="inlineStr">
@@ -21891,7 +21891,7 @@
       </c>
       <c r="I371" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J371" t="inlineStr">
@@ -21948,7 +21948,7 @@
       </c>
       <c r="I372" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J372" t="inlineStr">
@@ -22062,7 +22062,7 @@
       </c>
       <c r="I374" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J374" t="inlineStr">
@@ -22119,7 +22119,7 @@
       </c>
       <c r="I375" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J375" t="inlineStr">
@@ -22176,7 +22176,7 @@
       </c>
       <c r="I376" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J376" t="inlineStr">
@@ -22233,7 +22233,7 @@
       </c>
       <c r="I377" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="J377" t="inlineStr">
@@ -22290,7 +22290,7 @@
       </c>
       <c r="I378" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J378" t="inlineStr">
@@ -22347,7 +22347,7 @@
       </c>
       <c r="I379" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="J379" t="inlineStr">
@@ -22404,7 +22404,7 @@
       </c>
       <c r="I380" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J380" t="inlineStr">
@@ -22461,7 +22461,7 @@
       </c>
       <c r="I381" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J381" t="inlineStr">
@@ -22518,7 +22518,7 @@
       </c>
       <c r="I382" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J382" t="inlineStr">
@@ -22575,7 +22575,7 @@
       </c>
       <c r="I383" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J383" t="inlineStr">
@@ -22632,7 +22632,7 @@
       </c>
       <c r="I384" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="J384" t="inlineStr">
@@ -22689,7 +22689,7 @@
       </c>
       <c r="I385" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J385" t="inlineStr">
@@ -22746,7 +22746,7 @@
       </c>
       <c r="I386" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J386" t="inlineStr">
@@ -22860,7 +22860,7 @@
       </c>
       <c r="I388" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J388" t="inlineStr">
@@ -22917,7 +22917,7 @@
       </c>
       <c r="I389" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J389" t="inlineStr">
@@ -22974,7 +22974,7 @@
       </c>
       <c r="I390" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J390" t="inlineStr">
@@ -23031,7 +23031,7 @@
       </c>
       <c r="I391" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J391" t="inlineStr">
@@ -23088,7 +23088,7 @@
       </c>
       <c r="I392" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J392" t="inlineStr">
@@ -23145,7 +23145,7 @@
       </c>
       <c r="I393" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J393" t="inlineStr">
@@ -23202,7 +23202,7 @@
       </c>
       <c r="I394" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J394" t="inlineStr">
@@ -23259,7 +23259,7 @@
       </c>
       <c r="I395" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J395" t="inlineStr">
@@ -23316,7 +23316,7 @@
       </c>
       <c r="I396" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J396" t="inlineStr">
@@ -23373,7 +23373,7 @@
       </c>
       <c r="I397" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J397" t="inlineStr">

</xml_diff>

<commit_message>
Update charts, reports, and add original Pulse Dashboard prompt
Updated SLA/efficiency/executive chart PNGs with corrected financial
data, refreshed Strategic_Report.xlsx and classification_feedback.xlsx,
and added the original Pulse Dashboard build prompt for reference.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/classification_feedback.xlsx
+++ b/classification_feedback.xlsx
@@ -705,7 +705,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Generated: 2026-02-09 10:46</t>
+          <t>Generated: 2026-02-10 11:44</t>
         </is>
       </c>
     </row>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>29%</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -9408,7 +9408,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
@@ -9522,7 +9522,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J154" t="inlineStr">
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -12771,7 +12771,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="J211" t="inlineStr">
@@ -12942,7 +12942,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J214" t="inlineStr">
@@ -13170,7 +13170,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J218" t="inlineStr">
@@ -13227,7 +13227,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J219" t="inlineStr">
@@ -14880,7 +14880,7 @@
       </c>
       <c r="I248" t="inlineStr">
         <is>
-          <t>20%</t>
+          <t>21%</t>
         </is>
       </c>
       <c r="J248" t="inlineStr">
@@ -20181,7 +20181,7 @@
       </c>
       <c r="I341" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J341" t="inlineStr">
@@ -20238,7 +20238,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J342" t="inlineStr">
@@ -21435,7 +21435,7 @@
       </c>
       <c r="I363" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J363" t="inlineStr">

</xml_diff>

<commit_message>
Update chart images and report data files
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/classification_feedback.xlsx
+++ b/classification_feedback.xlsx
@@ -705,7 +705,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Generated: 2026-02-11 15:57</t>
+          <t>Generated: 2026-02-11 16:48</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -915,7 +915,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>32%</t>
+          <t>36%</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>18%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2055,7 +2055,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2283,7 +2283,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2340,7 +2340,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>11%</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3247,12 +3247,12 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>🟢 Low (&lt;30%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>29%</t>
+          <t>36%</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>13%</t>
+          <t>12%</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -3423,7 +3423,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3480,7 +3480,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3537,7 +3537,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>11%</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>12%</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -3765,7 +3765,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -4050,7 +4050,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -4107,7 +4107,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -4221,7 +4221,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -4449,7 +4449,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
@@ -4506,7 +4506,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -4677,7 +4677,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -4734,7 +4734,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -4791,7 +4791,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
@@ -4905,7 +4905,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -5076,7 +5076,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -5133,7 +5133,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
@@ -5190,7 +5190,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
@@ -5247,7 +5247,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
@@ -5304,7 +5304,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -5361,7 +5361,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -5475,7 +5475,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
@@ -5532,7 +5532,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
@@ -5646,7 +5646,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -5760,7 +5760,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
@@ -5817,7 +5817,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
@@ -5874,7 +5874,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
@@ -5931,7 +5931,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
@@ -6045,7 +6045,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -6216,7 +6216,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -6330,7 +6330,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -6387,7 +6387,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -6444,7 +6444,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>99%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -6558,7 +6558,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
@@ -6615,7 +6615,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
@@ -6672,7 +6672,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
@@ -6729,7 +6729,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
@@ -6786,7 +6786,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -6843,7 +6843,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
@@ -6900,7 +6900,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
@@ -6957,7 +6957,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
@@ -7014,7 +7014,7 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
@@ -7071,7 +7071,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
@@ -7128,7 +7128,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J112" t="inlineStr">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J113" t="inlineStr">
@@ -7242,7 +7242,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
@@ -7299,7 +7299,7 @@
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J115" t="inlineStr">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
@@ -7527,7 +7527,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J119" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -7641,7 +7641,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J121" t="inlineStr">
@@ -7698,7 +7698,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J122" t="inlineStr">
@@ -7755,7 +7755,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -7812,7 +7812,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -7869,7 +7869,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J125" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
@@ -7983,7 +7983,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J127" t="inlineStr">
@@ -8040,7 +8040,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
@@ -8097,7 +8097,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
@@ -8154,7 +8154,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J131" t="inlineStr">
@@ -8268,7 +8268,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J132" t="inlineStr">
@@ -8325,7 +8325,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J133" t="inlineStr">
@@ -8382,7 +8382,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J134" t="inlineStr">
@@ -8439,7 +8439,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
@@ -8496,7 +8496,7 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J136" t="inlineStr">
@@ -8553,7 +8553,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J137" t="inlineStr">
@@ -8610,7 +8610,7 @@
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J138" t="inlineStr">
@@ -8667,7 +8667,7 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J139" t="inlineStr">
@@ -8724,7 +8724,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J140" t="inlineStr">
@@ -8781,7 +8781,7 @@
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J141" t="inlineStr">
@@ -8895,7 +8895,7 @@
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -8952,7 +8952,7 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
@@ -9009,7 +9009,7 @@
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J145" t="inlineStr">
@@ -9066,7 +9066,7 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J146" t="inlineStr">
@@ -9123,7 +9123,7 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J147" t="inlineStr">
@@ -9180,7 +9180,7 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J148" t="inlineStr">
@@ -9237,7 +9237,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J149" t="inlineStr">
@@ -9294,7 +9294,7 @@
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J150" t="inlineStr">
@@ -9351,7 +9351,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J151" t="inlineStr">
@@ -9408,7 +9408,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
@@ -9465,7 +9465,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
@@ -9579,7 +9579,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J155" t="inlineStr">
@@ -9636,7 +9636,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
@@ -9693,7 +9693,7 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
@@ -9750,7 +9750,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>35%</t>
+          <t>36%</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
@@ -9807,7 +9807,7 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
@@ -9921,7 +9921,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
@@ -10035,7 +10035,7 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
@@ -10149,7 +10149,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
@@ -10263,7 +10263,7 @@
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J167" t="inlineStr">
@@ -10320,7 +10320,7 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
@@ -10377,7 +10377,7 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
@@ -10434,7 +10434,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
@@ -10548,7 +10548,7 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J172" t="inlineStr">
@@ -10662,7 +10662,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
@@ -10719,7 +10719,7 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J175" t="inlineStr">
@@ -10776,7 +10776,7 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J176" t="inlineStr">
@@ -10833,7 +10833,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
@@ -10890,7 +10890,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
@@ -10947,7 +10947,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
@@ -11004,7 +11004,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
@@ -11175,7 +11175,7 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
@@ -11232,7 +11232,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
@@ -11289,7 +11289,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
@@ -11346,7 +11346,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
@@ -11460,7 +11460,7 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
@@ -11517,7 +11517,7 @@
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J189" t="inlineStr">
@@ -11574,7 +11574,7 @@
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J190" t="inlineStr">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -11688,7 +11688,7 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J192" t="inlineStr">
@@ -11745,7 +11745,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
@@ -11802,7 +11802,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
@@ -11859,7 +11859,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
@@ -11916,7 +11916,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
@@ -11973,7 +11973,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
@@ -12030,7 +12030,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J198" t="inlineStr">
@@ -12144,7 +12144,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J200" t="inlineStr">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J201" t="inlineStr">
@@ -12258,7 +12258,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J202" t="inlineStr">
@@ -12315,7 +12315,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J203" t="inlineStr">
@@ -12372,7 +12372,7 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J204" t="inlineStr">
@@ -12429,7 +12429,7 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J205" t="inlineStr">
@@ -12486,7 +12486,7 @@
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J206" t="inlineStr">
@@ -12543,7 +12543,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J207" t="inlineStr">
@@ -12600,7 +12600,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J208" t="inlineStr">
@@ -12771,7 +12771,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="J211" t="inlineStr">
@@ -12828,7 +12828,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>38%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="J212" t="inlineStr">
@@ -12885,7 +12885,7 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J213" t="inlineStr">
@@ -12942,7 +12942,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>22%</t>
         </is>
       </c>
       <c r="J214" t="inlineStr">
@@ -12999,7 +12999,7 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J215" t="inlineStr">
@@ -13056,7 +13056,7 @@
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="J216" t="inlineStr">
@@ -13170,7 +13170,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J218" t="inlineStr">
@@ -13227,7 +13227,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J219" t="inlineStr">
@@ -13284,7 +13284,7 @@
       </c>
       <c r="I220" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J220" t="inlineStr">
@@ -13341,7 +13341,7 @@
       </c>
       <c r="I221" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J221" t="inlineStr">
@@ -13398,7 +13398,7 @@
       </c>
       <c r="I222" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J222" t="inlineStr">
@@ -13455,7 +13455,7 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J223" t="inlineStr">
@@ -13512,7 +13512,7 @@
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J224" t="inlineStr">
@@ -13569,7 +13569,7 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J225" t="inlineStr">
@@ -13626,7 +13626,7 @@
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>23%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="J226" t="inlineStr">
@@ -13740,7 +13740,7 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J228" t="inlineStr">
@@ -13797,7 +13797,7 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J229" t="inlineStr">
@@ -13854,7 +13854,7 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J230" t="inlineStr">
@@ -13911,7 +13911,7 @@
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J231" t="inlineStr">
@@ -13968,7 +13968,7 @@
       </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J232" t="inlineStr">
@@ -14025,7 +14025,7 @@
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J233" t="inlineStr">
@@ -14082,7 +14082,7 @@
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J234" t="inlineStr">
@@ -14139,7 +14139,7 @@
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J235" t="inlineStr">
@@ -14196,7 +14196,7 @@
       </c>
       <c r="I236" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J236" t="inlineStr">
@@ -14253,7 +14253,7 @@
       </c>
       <c r="I237" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J237" t="inlineStr">
@@ -14310,7 +14310,7 @@
       </c>
       <c r="I238" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J238" t="inlineStr">
@@ -14367,7 +14367,7 @@
       </c>
       <c r="I239" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J239" t="inlineStr">
@@ -14424,7 +14424,7 @@
       </c>
       <c r="I240" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J240" t="inlineStr">
@@ -14481,7 +14481,7 @@
       </c>
       <c r="I241" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="J241" t="inlineStr">
@@ -14538,7 +14538,7 @@
       </c>
       <c r="I242" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J242" t="inlineStr">
@@ -14595,7 +14595,7 @@
       </c>
       <c r="I243" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J243" t="inlineStr">
@@ -14652,7 +14652,7 @@
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J244" t="inlineStr">
@@ -14709,7 +14709,7 @@
       </c>
       <c r="I245" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J245" t="inlineStr">
@@ -14766,7 +14766,7 @@
       </c>
       <c r="I246" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J246" t="inlineStr">
@@ -14823,7 +14823,7 @@
       </c>
       <c r="I247" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J247" t="inlineStr">
@@ -14880,7 +14880,7 @@
       </c>
       <c r="I248" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J248" t="inlineStr">
@@ -14994,7 +14994,7 @@
       </c>
       <c r="I250" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J250" t="inlineStr">
@@ -15165,7 +15165,7 @@
       </c>
       <c r="I253" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J253" t="inlineStr">
@@ -15222,7 +15222,7 @@
       </c>
       <c r="I254" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J254" t="inlineStr">
@@ -15336,7 +15336,7 @@
       </c>
       <c r="I256" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J256" t="inlineStr">
@@ -15393,7 +15393,7 @@
       </c>
       <c r="I257" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J257" t="inlineStr">
@@ -15450,7 +15450,7 @@
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J258" t="inlineStr">
@@ -15507,7 +15507,7 @@
       </c>
       <c r="I259" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J259" t="inlineStr">
@@ -15564,7 +15564,7 @@
       </c>
       <c r="I260" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J260" t="inlineStr">
@@ -15621,7 +15621,7 @@
       </c>
       <c r="I261" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J261" t="inlineStr">
@@ -15678,7 +15678,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
@@ -15735,7 +15735,7 @@
       </c>
       <c r="I263" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>26%</t>
         </is>
       </c>
       <c r="J263" t="inlineStr">
@@ -15792,7 +15792,7 @@
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J264" t="inlineStr">
@@ -15906,7 +15906,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J266" t="inlineStr">
@@ -16077,7 +16077,7 @@
       </c>
       <c r="I269" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J269" t="inlineStr">
@@ -16134,7 +16134,7 @@
       </c>
       <c r="I270" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J270" t="inlineStr">
@@ -16191,7 +16191,7 @@
       </c>
       <c r="I271" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J271" t="inlineStr">
@@ -16248,7 +16248,7 @@
       </c>
       <c r="I272" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J272" t="inlineStr">
@@ -16305,7 +16305,7 @@
       </c>
       <c r="I273" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J273" t="inlineStr">
@@ -16362,7 +16362,7 @@
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J274" t="inlineStr">
@@ -16419,7 +16419,7 @@
       </c>
       <c r="I275" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J275" t="inlineStr">
@@ -16476,7 +16476,7 @@
       </c>
       <c r="I276" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J276" t="inlineStr">
@@ -16590,7 +16590,7 @@
       </c>
       <c r="I278" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J278" t="inlineStr">
@@ -16704,7 +16704,7 @@
       </c>
       <c r="I280" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J280" t="inlineStr">
@@ -16932,7 +16932,7 @@
       </c>
       <c r="I284" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J284" t="inlineStr">
@@ -17103,7 +17103,7 @@
       </c>
       <c r="I287" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J287" t="inlineStr">
@@ -17160,7 +17160,7 @@
       </c>
       <c r="I288" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J288" t="inlineStr">
@@ -17217,7 +17217,7 @@
       </c>
       <c r="I289" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J289" t="inlineStr">
@@ -17274,7 +17274,7 @@
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="J290" t="inlineStr">
@@ -17331,7 +17331,7 @@
       </c>
       <c r="I291" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J291" t="inlineStr">
@@ -17388,7 +17388,7 @@
       </c>
       <c r="I292" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J292" t="inlineStr">
@@ -17445,7 +17445,7 @@
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J293" t="inlineStr">
@@ -17502,7 +17502,7 @@
       </c>
       <c r="I294" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>37%</t>
         </is>
       </c>
       <c r="J294" t="inlineStr">
@@ -17616,7 +17616,7 @@
       </c>
       <c r="I296" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J296" t="inlineStr">
@@ -17673,7 +17673,7 @@
       </c>
       <c r="I297" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J297" t="inlineStr">
@@ -17730,7 +17730,7 @@
       </c>
       <c r="I298" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J298" t="inlineStr">
@@ -17787,7 +17787,7 @@
       </c>
       <c r="I299" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J299" t="inlineStr">
@@ -17844,7 +17844,7 @@
       </c>
       <c r="I300" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J300" t="inlineStr">
@@ -17901,7 +17901,7 @@
       </c>
       <c r="I301" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J301" t="inlineStr">
@@ -17958,7 +17958,7 @@
       </c>
       <c r="I302" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J302" t="inlineStr">
@@ -18015,7 +18015,7 @@
       </c>
       <c r="I303" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="J303" t="inlineStr">
@@ -18072,7 +18072,7 @@
       </c>
       <c r="I304" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="J304" t="inlineStr">
@@ -18129,7 +18129,7 @@
       </c>
       <c r="I305" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J305" t="inlineStr">
@@ -18186,7 +18186,7 @@
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J306" t="inlineStr">
@@ -18243,7 +18243,7 @@
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J307" t="inlineStr">
@@ -18300,7 +18300,7 @@
       </c>
       <c r="I308" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J308" t="inlineStr">
@@ -18357,7 +18357,7 @@
       </c>
       <c r="I309" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J309" t="inlineStr">
@@ -18414,7 +18414,7 @@
       </c>
       <c r="I310" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J310" t="inlineStr">
@@ -18471,7 +18471,7 @@
       </c>
       <c r="I311" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J311" t="inlineStr">
@@ -18528,7 +18528,7 @@
       </c>
       <c r="I312" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>24%</t>
         </is>
       </c>
       <c r="J312" t="inlineStr">
@@ -18585,7 +18585,7 @@
       </c>
       <c r="I313" t="inlineStr">
         <is>
-          <t>26%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J313" t="inlineStr">
@@ -18642,7 +18642,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J314" t="inlineStr">
@@ -18699,7 +18699,7 @@
       </c>
       <c r="I315" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J315" t="inlineStr">
@@ -18756,7 +18756,7 @@
       </c>
       <c r="I316" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J316" t="inlineStr">
@@ -18927,7 +18927,7 @@
       </c>
       <c r="I319" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J319" t="inlineStr">
@@ -19041,7 +19041,7 @@
       </c>
       <c r="I321" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J321" t="inlineStr">
@@ -19098,7 +19098,7 @@
       </c>
       <c r="I322" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J322" t="inlineStr">
@@ -19155,7 +19155,7 @@
       </c>
       <c r="I323" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="J323" t="inlineStr">
@@ -19212,7 +19212,7 @@
       </c>
       <c r="I324" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J324" t="inlineStr">
@@ -19269,7 +19269,7 @@
       </c>
       <c r="I325" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J325" t="inlineStr">
@@ -19321,12 +19321,12 @@
       </c>
       <c r="H326" t="inlineStr">
         <is>
-          <t>🟢 Low (&lt;30%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I326" t="inlineStr">
         <is>
-          <t>29%</t>
+          <t>31%</t>
         </is>
       </c>
       <c r="J326" t="inlineStr">
@@ -19383,7 +19383,7 @@
       </c>
       <c r="I327" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="J327" t="inlineStr">
@@ -19440,7 +19440,7 @@
       </c>
       <c r="I328" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J328" t="inlineStr">
@@ -19554,7 +19554,7 @@
       </c>
       <c r="I330" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J330" t="inlineStr">
@@ -19611,7 +19611,7 @@
       </c>
       <c r="I331" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J331" t="inlineStr">
@@ -19668,7 +19668,7 @@
       </c>
       <c r="I332" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J332" t="inlineStr">
@@ -19720,12 +19720,12 @@
       </c>
       <c r="H333" t="inlineStr">
         <is>
-          <t>🟢 Low (&lt;30%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I333" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>32%</t>
         </is>
       </c>
       <c r="J333" t="inlineStr">
@@ -19782,7 +19782,7 @@
       </c>
       <c r="I334" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="J334" t="inlineStr">
@@ -19834,12 +19834,12 @@
       </c>
       <c r="H335" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟠 Elevated (50-70%)</t>
         </is>
       </c>
       <c r="I335" t="inlineStr">
         <is>
-          <t>71%</t>
+          <t>67%</t>
         </is>
       </c>
       <c r="J335" t="inlineStr">
@@ -20010,7 +20010,7 @@
       </c>
       <c r="I338" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J338" t="inlineStr">
@@ -20067,7 +20067,7 @@
       </c>
       <c r="I339" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J339" t="inlineStr">
@@ -20124,7 +20124,7 @@
       </c>
       <c r="I340" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J340" t="inlineStr">
@@ -20181,7 +20181,7 @@
       </c>
       <c r="I341" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J341" t="inlineStr">
@@ -20238,7 +20238,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J342" t="inlineStr">
@@ -20295,7 +20295,7 @@
       </c>
       <c r="I343" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J343" t="inlineStr">
@@ -20352,7 +20352,7 @@
       </c>
       <c r="I344" t="inlineStr">
         <is>
-          <t>16%</t>
+          <t>19%</t>
         </is>
       </c>
       <c r="J344" t="inlineStr">
@@ -20409,7 +20409,7 @@
       </c>
       <c r="I345" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>16%</t>
         </is>
       </c>
       <c r="J345" t="inlineStr">
@@ -20466,7 +20466,7 @@
       </c>
       <c r="I346" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J346" t="inlineStr">
@@ -20523,7 +20523,7 @@
       </c>
       <c r="I347" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J347" t="inlineStr">
@@ -20575,7 +20575,7 @@
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>🔴 High Risk (&gt;70%)</t>
+          <t>🟠 Elevated (50-70%)</t>
         </is>
       </c>
       <c r="I348" t="inlineStr">
@@ -20637,7 +20637,7 @@
       </c>
       <c r="I349" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J349" t="inlineStr">
@@ -20694,7 +20694,7 @@
       </c>
       <c r="I350" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J350" t="inlineStr">
@@ -20751,7 +20751,7 @@
       </c>
       <c r="I351" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J351" t="inlineStr">
@@ -20917,12 +20917,12 @@
       </c>
       <c r="H354" t="inlineStr">
         <is>
-          <t>🟢 Low (&lt;30%)</t>
+          <t>🟡 Moderate (30-50%)</t>
         </is>
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t>24%</t>
+          <t>32%</t>
         </is>
       </c>
       <c r="J354" t="inlineStr">
@@ -20979,7 +20979,7 @@
       </c>
       <c r="I355" t="inlineStr">
         <is>
-          <t>22%</t>
+          <t>23%</t>
         </is>
       </c>
       <c r="J355" t="inlineStr">
@@ -21036,7 +21036,7 @@
       </c>
       <c r="I356" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J356" t="inlineStr">
@@ -21093,7 +21093,7 @@
       </c>
       <c r="I357" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="J357" t="inlineStr">
@@ -21150,7 +21150,7 @@
       </c>
       <c r="I358" t="inlineStr">
         <is>
-          <t>97%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J358" t="inlineStr">
@@ -21207,7 +21207,7 @@
       </c>
       <c r="I359" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J359" t="inlineStr">
@@ -21264,7 +21264,7 @@
       </c>
       <c r="I360" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J360" t="inlineStr">
@@ -21321,7 +21321,7 @@
       </c>
       <c r="I361" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="J361" t="inlineStr">
@@ -21378,7 +21378,7 @@
       </c>
       <c r="I362" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J362" t="inlineStr">
@@ -21492,7 +21492,7 @@
       </c>
       <c r="I364" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J364" t="inlineStr">
@@ -21549,7 +21549,7 @@
       </c>
       <c r="I365" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J365" t="inlineStr">
@@ -21606,7 +21606,7 @@
       </c>
       <c r="I366" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J366" t="inlineStr">
@@ -21663,7 +21663,7 @@
       </c>
       <c r="I367" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J367" t="inlineStr">
@@ -21720,7 +21720,7 @@
       </c>
       <c r="I368" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="J368" t="inlineStr">
@@ -21777,7 +21777,7 @@
       </c>
       <c r="I369" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J369" t="inlineStr">
@@ -21834,7 +21834,7 @@
       </c>
       <c r="I370" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J370" t="inlineStr">
@@ -21891,7 +21891,7 @@
       </c>
       <c r="I371" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J371" t="inlineStr">
@@ -21948,7 +21948,7 @@
       </c>
       <c r="I372" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J372" t="inlineStr">
@@ -22062,7 +22062,7 @@
       </c>
       <c r="I374" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J374" t="inlineStr">
@@ -22119,7 +22119,7 @@
       </c>
       <c r="I375" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J375" t="inlineStr">
@@ -22176,7 +22176,7 @@
       </c>
       <c r="I376" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J376" t="inlineStr">
@@ -22233,7 +22233,7 @@
       </c>
       <c r="I377" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="J377" t="inlineStr">
@@ -22290,7 +22290,7 @@
       </c>
       <c r="I378" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J378" t="inlineStr">
@@ -22347,7 +22347,7 @@
       </c>
       <c r="I379" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="J379" t="inlineStr">
@@ -22404,7 +22404,7 @@
       </c>
       <c r="I380" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J380" t="inlineStr">
@@ -22461,7 +22461,7 @@
       </c>
       <c r="I381" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J381" t="inlineStr">
@@ -22518,7 +22518,7 @@
       </c>
       <c r="I382" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>97%</t>
         </is>
       </c>
       <c r="J382" t="inlineStr">
@@ -22575,7 +22575,7 @@
       </c>
       <c r="I383" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="J383" t="inlineStr">
@@ -22632,7 +22632,7 @@
       </c>
       <c r="I384" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="J384" t="inlineStr">
@@ -22689,7 +22689,7 @@
       </c>
       <c r="I385" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="J385" t="inlineStr">
@@ -22746,7 +22746,7 @@
       </c>
       <c r="I386" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J386" t="inlineStr">
@@ -22860,7 +22860,7 @@
       </c>
       <c r="I388" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J388" t="inlineStr">
@@ -22917,7 +22917,7 @@
       </c>
       <c r="I389" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="J389" t="inlineStr">
@@ -22974,7 +22974,7 @@
       </c>
       <c r="I390" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="J390" t="inlineStr">
@@ -23031,7 +23031,7 @@
       </c>
       <c r="I391" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J391" t="inlineStr">
@@ -23088,7 +23088,7 @@
       </c>
       <c r="I392" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>99%</t>
         </is>
       </c>
       <c r="J392" t="inlineStr">
@@ -23145,7 +23145,7 @@
       </c>
       <c r="I393" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="J393" t="inlineStr">
@@ -23202,7 +23202,7 @@
       </c>
       <c r="I394" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="J394" t="inlineStr">
@@ -23259,7 +23259,7 @@
       </c>
       <c r="I395" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="J395" t="inlineStr">
@@ -23316,7 +23316,7 @@
       </c>
       <c r="I396" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="J396" t="inlineStr">
@@ -23373,7 +23373,7 @@
       </c>
       <c r="I397" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="J397" t="inlineStr">

</xml_diff>